<commit_message>
Various changes: - run for many time periods - parametrisation - changed benchmarking - added plots - applied tryCatch to Bayesian and Conformal Prediction
</commit_message>
<xml_diff>
--- a/Analysis drafts/Miscellaneous/Approach CP und QR.xlsx
+++ b/Analysis drafts/Miscellaneous/Approach CP und QR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Studium\Master\Université de Genève\Kurse\Master thesis\Drafts\Analysis drafts\Miscellaneous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656EBD53-59E8-428C-A8B4-D371B5CA0B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F521399F-CCAE-47F5-BEB5-4653C920B477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10870" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{8027843B-AE8F-422B-8197-31000C3E0078}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{8027843B-AE8F-422B-8197-31000C3E0078}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="99">
   <si>
     <t>Id</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>Again, introducing a small tolerance for the lower boundary makes sense</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -929,7 +932,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1089,6 +1092,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1158,16 +1162,16 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1197,10 +1201,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1395,8 +1395,8 @@
       <xdr:rowOff>181610</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1891993" cy="165366"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1542,7 +1542,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1745,8 +1745,8 @@
       <xdr:rowOff>161290</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2763192" cy="173766"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -1793,6 +1793,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1870,7 +1871,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -4561,17 +4562,17 @@
       <c r="I4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="121" t="s">
+      <c r="J4" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="121"/>
-      <c r="L4" s="121"/>
+      <c r="K4" s="122"/>
+      <c r="L4" s="122"/>
     </row>
     <row r="5" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="129" t="s">
+      <c r="B5" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="132" t="s">
+      <c r="C5" s="133" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2">
@@ -4592,15 +4593,15 @@
       <c r="I5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="135" t="s">
+      <c r="J5" s="136" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="135"/>
-      <c r="L5" s="135"/>
+      <c r="K5" s="136"/>
+      <c r="L5" s="136"/>
     </row>
     <row r="6" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="130"/>
-      <c r="C6" s="133"/>
+      <c r="B6" s="131"/>
+      <c r="C6" s="134"/>
       <c r="D6" s="2">
         <v>2</v>
       </c>
@@ -4619,13 +4620,13 @@
       <c r="I6" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="128"/>
-      <c r="K6" s="128"/>
-      <c r="L6" s="128"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="129"/>
+      <c r="L6" s="129"/>
     </row>
     <row r="7" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="130"/>
-      <c r="C7" s="133"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="134"/>
       <c r="D7" s="2">
         <v>3</v>
       </c>
@@ -4644,13 +4645,13 @@
       <c r="I7" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="128"/>
-      <c r="K7" s="128"/>
-      <c r="L7" s="128"/>
+      <c r="J7" s="129"/>
+      <c r="K7" s="129"/>
+      <c r="L7" s="129"/>
     </row>
     <row r="8" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="130"/>
-      <c r="C8" s="133"/>
+      <c r="B8" s="131"/>
+      <c r="C8" s="134"/>
       <c r="D8" s="2">
         <v>4</v>
       </c>
@@ -4669,13 +4670,13 @@
       <c r="I8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="128"/>
-      <c r="K8" s="128"/>
-      <c r="L8" s="128"/>
+      <c r="J8" s="129"/>
+      <c r="K8" s="129"/>
+      <c r="L8" s="129"/>
     </row>
     <row r="9" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="130"/>
-      <c r="C9" s="133"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="134"/>
       <c r="D9" s="2">
         <v>5</v>
       </c>
@@ -4694,13 +4695,13 @@
       <c r="I9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="128"/>
-      <c r="K9" s="128"/>
-      <c r="L9" s="128"/>
+      <c r="J9" s="129"/>
+      <c r="K9" s="129"/>
+      <c r="L9" s="129"/>
     </row>
     <row r="10" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="130"/>
-      <c r="C10" s="133"/>
+      <c r="B10" s="131"/>
+      <c r="C10" s="134"/>
       <c r="D10" s="2">
         <v>6</v>
       </c>
@@ -4719,13 +4720,13 @@
       <c r="I10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="128"/>
-      <c r="K10" s="128"/>
-      <c r="L10" s="128"/>
+      <c r="J10" s="129"/>
+      <c r="K10" s="129"/>
+      <c r="L10" s="129"/>
     </row>
     <row r="11" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="130"/>
-      <c r="C11" s="133"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="134"/>
       <c r="D11" s="2">
         <v>7</v>
       </c>
@@ -4744,13 +4745,13 @@
       <c r="I11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="128"/>
-      <c r="K11" s="128"/>
-      <c r="L11" s="128"/>
+      <c r="J11" s="129"/>
+      <c r="K11" s="129"/>
+      <c r="L11" s="129"/>
     </row>
     <row r="12" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="130"/>
-      <c r="C12" s="133"/>
+      <c r="B12" s="131"/>
+      <c r="C12" s="134"/>
       <c r="D12" s="2">
         <v>8</v>
       </c>
@@ -4769,13 +4770,13 @@
       <c r="I12" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="128"/>
-      <c r="K12" s="128"/>
-      <c r="L12" s="128"/>
+      <c r="J12" s="129"/>
+      <c r="K12" s="129"/>
+      <c r="L12" s="129"/>
     </row>
     <row r="13" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="130"/>
-      <c r="C13" s="133"/>
+      <c r="B13" s="131"/>
+      <c r="C13" s="134"/>
       <c r="D13" s="2">
         <v>9</v>
       </c>
@@ -4794,13 +4795,13 @@
       <c r="I13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="128"/>
-      <c r="K13" s="128"/>
-      <c r="L13" s="128"/>
+      <c r="J13" s="129"/>
+      <c r="K13" s="129"/>
+      <c r="L13" s="129"/>
     </row>
     <row r="14" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="130"/>
-      <c r="C14" s="133"/>
+      <c r="B14" s="131"/>
+      <c r="C14" s="134"/>
       <c r="D14" s="2">
         <v>10</v>
       </c>
@@ -4819,13 +4820,13 @@
       <c r="I14" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J14" s="128"/>
-      <c r="K14" s="128"/>
-      <c r="L14" s="128"/>
+      <c r="J14" s="129"/>
+      <c r="K14" s="129"/>
+      <c r="L14" s="129"/>
     </row>
     <row r="15" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="130"/>
-      <c r="C15" s="133"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="134"/>
       <c r="D15" s="2">
         <v>11</v>
       </c>
@@ -4844,13 +4845,13 @@
       <c r="I15" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J15" s="128"/>
-      <c r="K15" s="128"/>
-      <c r="L15" s="128"/>
+      <c r="J15" s="129"/>
+      <c r="K15" s="129"/>
+      <c r="L15" s="129"/>
     </row>
     <row r="16" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="130"/>
-      <c r="C16" s="133"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="134"/>
       <c r="D16" s="2">
         <v>12</v>
       </c>
@@ -4869,13 +4870,13 @@
       <c r="I16" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J16" s="128"/>
-      <c r="K16" s="128"/>
-      <c r="L16" s="128"/>
+      <c r="J16" s="129"/>
+      <c r="K16" s="129"/>
+      <c r="L16" s="129"/>
     </row>
     <row r="17" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="130"/>
-      <c r="C17" s="134"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="135"/>
       <c r="D17" s="2">
         <v>13</v>
       </c>
@@ -4894,12 +4895,12 @@
       <c r="I17" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="J17" s="128"/>
-      <c r="K17" s="128"/>
-      <c r="L17" s="128"/>
+      <c r="J17" s="129"/>
+      <c r="K17" s="129"/>
+      <c r="L17" s="129"/>
     </row>
     <row r="18" spans="2:14" s="2" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="130"/>
+      <c r="B18" s="131"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -4914,8 +4915,8 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="130"/>
-      <c r="C19" s="132" t="s">
+      <c r="B19" s="131"/>
+      <c r="C19" s="133" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="2">
@@ -4940,18 +4941,18 @@
         <f>ABS(H19-I19)</f>
         <v>1.0699999999999998</v>
       </c>
-      <c r="K19" s="128" t="s">
+      <c r="K19" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="L19" s="128"/>
+      <c r="L19" s="129"/>
       <c r="M19" s="2">
         <f>_xlfn.PERCENTILE.INC(J19:J30,0.9)</f>
         <v>15.029000000000002</v>
       </c>
     </row>
     <row r="20" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="130"/>
-      <c r="C20" s="133"/>
+      <c r="B20" s="131"/>
+      <c r="C20" s="134"/>
       <c r="D20" s="2">
         <v>15</v>
       </c>
@@ -4974,12 +4975,12 @@
         <f t="shared" ref="J20:J30" si="0">ABS(H20-I20)</f>
         <v>1.5700000000000003</v>
       </c>
-      <c r="K20" s="128"/>
-      <c r="L20" s="128"/>
+      <c r="K20" s="129"/>
+      <c r="L20" s="129"/>
     </row>
     <row r="21" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="130"/>
-      <c r="C21" s="133"/>
+      <c r="B21" s="131"/>
+      <c r="C21" s="134"/>
       <c r="D21" s="2">
         <v>16</v>
       </c>
@@ -5002,12 +5003,12 @@
         <f t="shared" si="0"/>
         <v>23.58</v>
       </c>
-      <c r="K21" s="128"/>
-      <c r="L21" s="128"/>
+      <c r="K21" s="129"/>
+      <c r="L21" s="129"/>
     </row>
     <row r="22" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="130"/>
-      <c r="C22" s="133"/>
+      <c r="B22" s="131"/>
+      <c r="C22" s="134"/>
       <c r="D22" s="2">
         <v>17</v>
       </c>
@@ -5030,12 +5031,12 @@
         <f t="shared" si="0"/>
         <v>4.25</v>
       </c>
-      <c r="K22" s="128"/>
-      <c r="L22" s="128"/>
+      <c r="K22" s="129"/>
+      <c r="L22" s="129"/>
     </row>
     <row r="23" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="130"/>
-      <c r="C23" s="133"/>
+      <c r="B23" s="131"/>
+      <c r="C23" s="134"/>
       <c r="D23" s="2">
         <v>18</v>
       </c>
@@ -5058,12 +5059,12 @@
         <f t="shared" si="0"/>
         <v>0.43</v>
       </c>
-      <c r="K23" s="128"/>
-      <c r="L23" s="128"/>
+      <c r="K23" s="129"/>
+      <c r="L23" s="129"/>
     </row>
     <row r="24" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="130"/>
-      <c r="C24" s="133"/>
+      <c r="B24" s="131"/>
+      <c r="C24" s="134"/>
       <c r="D24" s="2">
         <v>19</v>
       </c>
@@ -5086,12 +5087,12 @@
         <f t="shared" si="0"/>
         <v>3.95</v>
       </c>
-      <c r="K24" s="128"/>
-      <c r="L24" s="128"/>
+      <c r="K24" s="129"/>
+      <c r="L24" s="129"/>
     </row>
     <row r="25" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="130"/>
-      <c r="C25" s="133"/>
+      <c r="B25" s="131"/>
+      <c r="C25" s="134"/>
       <c r="D25" s="2">
         <v>20</v>
       </c>
@@ -5114,12 +5115,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="K25" s="128"/>
-      <c r="L25" s="128"/>
+      <c r="K25" s="129"/>
+      <c r="L25" s="129"/>
     </row>
     <row r="26" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="130"/>
-      <c r="C26" s="133"/>
+      <c r="B26" s="131"/>
+      <c r="C26" s="134"/>
       <c r="D26" s="2">
         <v>21</v>
       </c>
@@ -5142,12 +5143,12 @@
         <f t="shared" si="0"/>
         <v>8.9999999999999858E-2</v>
       </c>
-      <c r="K26" s="128"/>
-      <c r="L26" s="128"/>
+      <c r="K26" s="129"/>
+      <c r="L26" s="129"/>
     </row>
     <row r="27" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="130"/>
-      <c r="C27" s="133"/>
+      <c r="B27" s="131"/>
+      <c r="C27" s="134"/>
       <c r="D27" s="2">
         <v>22</v>
       </c>
@@ -5170,12 +5171,12 @@
         <f t="shared" si="0"/>
         <v>9.9799999999999986</v>
       </c>
-      <c r="K27" s="128"/>
-      <c r="L27" s="128"/>
+      <c r="K27" s="129"/>
+      <c r="L27" s="129"/>
     </row>
     <row r="28" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="130"/>
-      <c r="C28" s="133"/>
+      <c r="B28" s="131"/>
+      <c r="C28" s="134"/>
       <c r="D28" s="2">
         <v>23</v>
       </c>
@@ -5198,12 +5199,12 @@
         <f t="shared" si="0"/>
         <v>2.3899999999999997</v>
       </c>
-      <c r="K28" s="128"/>
-      <c r="L28" s="128"/>
+      <c r="K28" s="129"/>
+      <c r="L28" s="129"/>
     </row>
     <row r="29" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="130"/>
-      <c r="C29" s="133"/>
+      <c r="B29" s="131"/>
+      <c r="C29" s="134"/>
       <c r="D29" s="2">
         <v>24</v>
       </c>
@@ -5226,12 +5227,12 @@
         <f t="shared" si="0"/>
         <v>15.59</v>
       </c>
-      <c r="K29" s="128"/>
-      <c r="L29" s="128"/>
+      <c r="K29" s="129"/>
+      <c r="L29" s="129"/>
     </row>
     <row r="30" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="131"/>
-      <c r="C30" s="134"/>
+      <c r="B30" s="132"/>
+      <c r="C30" s="135"/>
       <c r="D30" s="2">
         <v>25</v>
       </c>
@@ -5254,8 +5255,8 @@
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="K30" s="128"/>
-      <c r="L30" s="128"/>
+      <c r="K30" s="129"/>
+      <c r="L30" s="129"/>
     </row>
     <row r="31" spans="2:14" s="2" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
@@ -5275,10 +5276,10 @@
       <c r="L31" s="4"/>
     </row>
     <row r="32" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="122" t="s">
+      <c r="B32" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="123"/>
+      <c r="C32" s="124"/>
       <c r="D32" s="2">
         <v>26</v>
       </c>
@@ -5304,15 +5305,15 @@
       <c r="K32" s="2">
         <v>1</v>
       </c>
-      <c r="L32" s="128" t="s">
+      <c r="L32" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="M32" s="128"/>
-      <c r="N32" s="128"/>
+      <c r="M32" s="129"/>
+      <c r="N32" s="129"/>
     </row>
     <row r="33" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="124"/>
-      <c r="C33" s="125"/>
+      <c r="B33" s="125"/>
+      <c r="C33" s="126"/>
       <c r="D33" s="2">
         <v>27</v>
       </c>
@@ -5338,13 +5339,13 @@
       <c r="K33" s="2">
         <v>1</v>
       </c>
-      <c r="L33" s="128"/>
-      <c r="M33" s="128"/>
-      <c r="N33" s="128"/>
+      <c r="L33" s="129"/>
+      <c r="M33" s="129"/>
+      <c r="N33" s="129"/>
     </row>
     <row r="34" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="124"/>
-      <c r="C34" s="125"/>
+      <c r="B34" s="125"/>
+      <c r="C34" s="126"/>
       <c r="D34" s="2">
         <v>28</v>
       </c>
@@ -5370,13 +5371,13 @@
       <c r="K34" s="2">
         <v>1</v>
       </c>
-      <c r="L34" s="128"/>
-      <c r="M34" s="128"/>
-      <c r="N34" s="128"/>
+      <c r="L34" s="129"/>
+      <c r="M34" s="129"/>
+      <c r="N34" s="129"/>
     </row>
     <row r="35" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="124"/>
-      <c r="C35" s="125"/>
+      <c r="B35" s="125"/>
+      <c r="C35" s="126"/>
       <c r="D35" s="2">
         <v>29</v>
       </c>
@@ -5402,13 +5403,13 @@
       <c r="K35" s="2">
         <v>0</v>
       </c>
-      <c r="L35" s="128"/>
-      <c r="M35" s="128"/>
-      <c r="N35" s="128"/>
+      <c r="L35" s="129"/>
+      <c r="M35" s="129"/>
+      <c r="N35" s="129"/>
     </row>
     <row r="36" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="124"/>
-      <c r="C36" s="125"/>
+      <c r="B36" s="125"/>
+      <c r="C36" s="126"/>
       <c r="D36" s="2">
         <v>30</v>
       </c>
@@ -5434,13 +5435,13 @@
       <c r="K36" s="2">
         <v>1</v>
       </c>
-      <c r="L36" s="128"/>
-      <c r="M36" s="128"/>
-      <c r="N36" s="128"/>
+      <c r="L36" s="129"/>
+      <c r="M36" s="129"/>
+      <c r="N36" s="129"/>
     </row>
     <row r="37" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="124"/>
-      <c r="C37" s="125"/>
+      <c r="B37" s="125"/>
+      <c r="C37" s="126"/>
       <c r="D37" s="2">
         <v>31</v>
       </c>
@@ -5466,13 +5467,13 @@
       <c r="K37" s="2">
         <v>1</v>
       </c>
-      <c r="L37" s="128"/>
-      <c r="M37" s="128"/>
-      <c r="N37" s="128"/>
+      <c r="L37" s="129"/>
+      <c r="M37" s="129"/>
+      <c r="N37" s="129"/>
     </row>
     <row r="38" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="126"/>
-      <c r="C38" s="127"/>
+      <c r="B38" s="127"/>
+      <c r="C38" s="128"/>
       <c r="D38" s="2">
         <v>32</v>
       </c>
@@ -5498,9 +5499,9 @@
       <c r="K38" s="2">
         <v>1</v>
       </c>
-      <c r="L38" s="128"/>
-      <c r="M38" s="128"/>
-      <c r="N38" s="128"/>
+      <c r="L38" s="129"/>
+      <c r="M38" s="129"/>
+      <c r="N38" s="129"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="K39">
@@ -5575,10 +5576,10 @@
       </c>
     </row>
     <row r="5" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="136" t="s">
+      <c r="B5" s="137" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="129" t="s">
+      <c r="C5" s="130" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="26">
@@ -5607,14 +5608,14 @@
         <f>ROUND(J5/(LM!B$17+LM!B$18*'CP 1'!I5),2)</f>
         <v>0.8</v>
       </c>
-      <c r="L5" s="137" t="s">
+      <c r="L5" s="138" t="s">
         <v>92</v>
       </c>
-      <c r="M5" s="137"/>
+      <c r="M5" s="138"/>
     </row>
     <row r="6" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="136"/>
-      <c r="C6" s="130"/>
+      <c r="B6" s="137"/>
+      <c r="C6" s="131"/>
       <c r="D6" s="28">
         <v>2</v>
       </c>
@@ -5641,12 +5642,12 @@
         <f>ROUND(J6/(LM!B$17+LM!B$18*'CP 1'!I6),2)</f>
         <v>1.03</v>
       </c>
-      <c r="L6" s="137"/>
-      <c r="M6" s="137"/>
+      <c r="L6" s="138"/>
+      <c r="M6" s="138"/>
     </row>
     <row r="7" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="136"/>
-      <c r="C7" s="130"/>
+      <c r="B7" s="137"/>
+      <c r="C7" s="131"/>
       <c r="D7" s="28">
         <v>3</v>
       </c>
@@ -5673,12 +5674,12 @@
         <f>ROUND(J7/(LM!B$17+LM!B$18*'CP 1'!I7),2)</f>
         <v>0.67</v>
       </c>
-      <c r="L7" s="137"/>
-      <c r="M7" s="137"/>
+      <c r="L7" s="138"/>
+      <c r="M7" s="138"/>
     </row>
     <row r="8" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="136"/>
-      <c r="C8" s="130"/>
+      <c r="B8" s="137"/>
+      <c r="C8" s="131"/>
       <c r="D8" s="28">
         <v>4</v>
       </c>
@@ -5705,12 +5706,12 @@
         <f>ROUND(J8/(LM!B$17+LM!B$18*'CP 1'!I8),2)</f>
         <v>0.12</v>
       </c>
-      <c r="L8" s="137"/>
-      <c r="M8" s="137"/>
+      <c r="L8" s="138"/>
+      <c r="M8" s="138"/>
     </row>
     <row r="9" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="136"/>
-      <c r="C9" s="130"/>
+      <c r="B9" s="137"/>
+      <c r="C9" s="131"/>
       <c r="D9" s="28">
         <v>5</v>
       </c>
@@ -5737,12 +5738,12 @@
         <f>ROUND(J9/(LM!B$17+LM!B$18*'CP 1'!I9),2)</f>
         <v>0.2</v>
       </c>
-      <c r="L9" s="137"/>
-      <c r="M9" s="137"/>
+      <c r="L9" s="138"/>
+      <c r="M9" s="138"/>
     </row>
     <row r="10" spans="2:17" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="136"/>
-      <c r="C10" s="130"/>
+      <c r="B10" s="137"/>
+      <c r="C10" s="131"/>
       <c r="D10" s="28">
         <v>6</v>
       </c>
@@ -5769,15 +5770,15 @@
         <f>ROUND(J10/(LM!B$17+LM!B$18*'CP 1'!I10),2)</f>
         <v>1.1399999999999999</v>
       </c>
-      <c r="L10" s="137"/>
-      <c r="M10" s="137"/>
+      <c r="L10" s="138"/>
+      <c r="M10" s="138"/>
       <c r="N10" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="136"/>
-      <c r="C11" s="130"/>
+      <c r="B11" s="137"/>
+      <c r="C11" s="131"/>
       <c r="D11" s="28">
         <v>7</v>
       </c>
@@ -5804,8 +5805,8 @@
         <f>ROUND(J11/(LM!B$17+LM!B$18*'CP 1'!I11),2)</f>
         <v>0.33</v>
       </c>
-      <c r="L11" s="137"/>
-      <c r="M11" s="137"/>
+      <c r="L11" s="138"/>
+      <c r="M11" s="138"/>
       <c r="N11" s="26" t="s">
         <v>19</v>
       </c>
@@ -5814,8 +5815,8 @@
       </c>
     </row>
     <row r="12" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="136"/>
-      <c r="C12" s="130"/>
+      <c r="B12" s="137"/>
+      <c r="C12" s="131"/>
       <c r="D12" s="28">
         <v>8</v>
       </c>
@@ -5842,8 +5843,8 @@
         <f>ROUND(J12/(LM!B$17+LM!B$18*'CP 1'!I12),2)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="L12" s="137"/>
-      <c r="M12" s="137"/>
+      <c r="L12" s="138"/>
+      <c r="M12" s="138"/>
       <c r="N12" s="28" t="s">
         <v>20</v>
       </c>
@@ -5852,8 +5853,8 @@
       </c>
     </row>
     <row r="13" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="136"/>
-      <c r="C13" s="130"/>
+      <c r="B13" s="137"/>
+      <c r="C13" s="131"/>
       <c r="D13" s="28">
         <v>9</v>
       </c>
@@ -5880,8 +5881,8 @@
         <f>ROUND(J13/(LM!B$17+LM!B$18*'CP 1'!I13),2)</f>
         <v>0.03</v>
       </c>
-      <c r="L13" s="137"/>
-      <c r="M13" s="137"/>
+      <c r="L13" s="138"/>
+      <c r="M13" s="138"/>
       <c r="N13" s="28" t="s">
         <v>21</v>
       </c>
@@ -5891,8 +5892,8 @@
       </c>
     </row>
     <row r="14" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="136"/>
-      <c r="C14" s="130"/>
+      <c r="B14" s="137"/>
+      <c r="C14" s="131"/>
       <c r="D14" s="28">
         <v>10</v>
       </c>
@@ -5919,8 +5920,8 @@
         <f>ROUND(J14/(LM!B$17+LM!B$18*'CP 1'!I14),2)</f>
         <v>0.69</v>
       </c>
-      <c r="L14" s="137"/>
-      <c r="M14" s="137"/>
+      <c r="L14" s="138"/>
+      <c r="M14" s="138"/>
       <c r="N14" s="28" t="s">
         <v>22</v>
       </c>
@@ -5929,8 +5930,8 @@
       </c>
     </row>
     <row r="15" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="136"/>
-      <c r="C15" s="130"/>
+      <c r="B15" s="137"/>
+      <c r="C15" s="131"/>
       <c r="D15" s="28">
         <v>11</v>
       </c>
@@ -5957,8 +5958,8 @@
         <f>ROUND(J15/(LM!B$17+LM!B$18*'CP 1'!I15),2)</f>
         <v>0.95</v>
       </c>
-      <c r="L15" s="137"/>
-      <c r="M15" s="137"/>
+      <c r="L15" s="138"/>
+      <c r="M15" s="138"/>
       <c r="N15" s="28" t="s">
         <v>22</v>
       </c>
@@ -5967,8 +5968,8 @@
       </c>
     </row>
     <row r="16" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="136"/>
-      <c r="C16" s="130"/>
+      <c r="B16" s="137"/>
+      <c r="C16" s="131"/>
       <c r="D16" s="28">
         <v>12</v>
       </c>
@@ -5995,8 +5996,8 @@
         <f>ROUND(J16/(LM!B$17+LM!B$18*'CP 1'!I16),2)</f>
         <v>0.56999999999999995</v>
       </c>
-      <c r="L16" s="137"/>
-      <c r="M16" s="137"/>
+      <c r="L16" s="138"/>
+      <c r="M16" s="138"/>
       <c r="N16" s="28" t="s">
         <v>22</v>
       </c>
@@ -6005,8 +6006,8 @@
       </c>
     </row>
     <row r="17" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="136"/>
-      <c r="C17" s="130"/>
+      <c r="B17" s="137"/>
+      <c r="C17" s="131"/>
       <c r="D17" s="28">
         <v>13</v>
       </c>
@@ -6033,8 +6034,8 @@
         <f>ROUND(J17/(LM!B$17+LM!B$18*'CP 1'!I17),2)</f>
         <v>0.83</v>
       </c>
-      <c r="L17" s="137"/>
-      <c r="M17" s="137"/>
+      <c r="L17" s="138"/>
+      <c r="M17" s="138"/>
       <c r="N17" s="28" t="s">
         <v>22</v>
       </c>
@@ -6043,8 +6044,8 @@
       </c>
     </row>
     <row r="18" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="136"/>
-      <c r="C18" s="130"/>
+      <c r="B18" s="137"/>
+      <c r="C18" s="131"/>
       <c r="D18" s="28">
         <v>14</v>
       </c>
@@ -6071,8 +6072,8 @@
         <f>ROUND(J18/(LM!B$17+LM!B$18*'CP 1'!I18),2)</f>
         <v>0.56999999999999995</v>
       </c>
-      <c r="L18" s="137"/>
-      <c r="M18" s="137"/>
+      <c r="L18" s="138"/>
+      <c r="M18" s="138"/>
       <c r="N18" s="30" t="s">
         <v>24</v>
       </c>
@@ -6081,8 +6082,8 @@
       </c>
     </row>
     <row r="19" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="136"/>
-      <c r="C19" s="130"/>
+      <c r="B19" s="137"/>
+      <c r="C19" s="131"/>
       <c r="D19" s="28">
         <v>15</v>
       </c>
@@ -6109,13 +6110,13 @@
         <f>ROUND(J19/(LM!B$17+LM!B$18*'CP 1'!I19),2)</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="L19" s="137"/>
-      <c r="M19" s="137"/>
+      <c r="L19" s="138"/>
+      <c r="M19" s="138"/>
       <c r="N19" s="25"/>
     </row>
     <row r="20" spans="2:20" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="136"/>
-      <c r="C20" s="131"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="132"/>
       <c r="D20" s="30">
         <v>16</v>
       </c>
@@ -6155,7 +6156,7 @@
       </c>
     </row>
     <row r="21" spans="2:20" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="136"/>
+      <c r="B21" s="137"/>
       <c r="I21" s="35"/>
       <c r="J21" s="53" t="s">
         <v>12</v>
@@ -6171,8 +6172,8 @@
       </c>
     </row>
     <row r="22" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="136"/>
-      <c r="C22" s="129" t="s">
+      <c r="B22" s="137"/>
+      <c r="C22" s="130" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="26">
@@ -6201,11 +6202,11 @@
         <f t="shared" ref="K22:K37" si="1">IF(AND(H22&gt;=S22,H22&lt;=T22),1,0)</f>
         <v>0</v>
       </c>
-      <c r="L22" s="137" t="s">
+      <c r="L22" s="138" t="s">
         <v>58</v>
       </c>
-      <c r="M22" s="137"/>
-      <c r="N22" s="137"/>
+      <c r="M22" s="138"/>
+      <c r="N22" s="138"/>
       <c r="O22" s="48"/>
       <c r="S22" s="1">
         <f>ROUND(MAX(0,I22-L$20*(LM!B$17+LM!B$18*'CP 1'!I22)),2)</f>
@@ -6217,8 +6218,8 @@
       </c>
     </row>
     <row r="23" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="136"/>
-      <c r="C23" s="130"/>
+      <c r="B23" s="137"/>
+      <c r="C23" s="131"/>
       <c r="D23" s="28">
         <v>18</v>
       </c>
@@ -6245,9 +6246,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L23" s="137"/>
-      <c r="M23" s="137"/>
-      <c r="N23" s="137"/>
+      <c r="L23" s="138"/>
+      <c r="M23" s="138"/>
+      <c r="N23" s="138"/>
       <c r="O23" s="48"/>
       <c r="S23" s="1">
         <f>ROUND(MAX(0,I23-L$20*(LM!B$17+LM!B$18*'CP 1'!I23)),2)</f>
@@ -6259,8 +6260,8 @@
       </c>
     </row>
     <row r="24" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="136"/>
-      <c r="C24" s="130"/>
+      <c r="B24" s="137"/>
+      <c r="C24" s="131"/>
       <c r="D24" s="28">
         <v>19</v>
       </c>
@@ -6287,9 +6288,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L24" s="137"/>
-      <c r="M24" s="137"/>
-      <c r="N24" s="137"/>
+      <c r="L24" s="138"/>
+      <c r="M24" s="138"/>
+      <c r="N24" s="138"/>
       <c r="O24" s="48"/>
       <c r="S24" s="1">
         <f>ROUND(MAX(0,I24-L$20*(LM!B$17+LM!B$18*'CP 1'!I24)),2)</f>
@@ -6301,8 +6302,8 @@
       </c>
     </row>
     <row r="25" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="136"/>
-      <c r="C25" s="130"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="131"/>
       <c r="D25" s="28">
         <v>20</v>
       </c>
@@ -6329,9 +6330,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L25" s="137"/>
-      <c r="M25" s="137"/>
-      <c r="N25" s="137"/>
+      <c r="L25" s="138"/>
+      <c r="M25" s="138"/>
+      <c r="N25" s="138"/>
       <c r="O25" s="48"/>
       <c r="S25" s="1">
         <f>ROUND(MAX(0,I25-L$20*(LM!B$17+LM!B$18*'CP 1'!I25)),2)</f>
@@ -6343,8 +6344,8 @@
       </c>
     </row>
     <row r="26" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="136"/>
-      <c r="C26" s="130"/>
+      <c r="B26" s="137"/>
+      <c r="C26" s="131"/>
       <c r="D26" s="28">
         <v>21</v>
       </c>
@@ -6371,9 +6372,9 @@
         <f>IF(AND(H26&gt;=S26,H26&lt;=T26),1,0)</f>
         <v>0</v>
       </c>
-      <c r="L26" s="137"/>
-      <c r="M26" s="137"/>
-      <c r="N26" s="137"/>
+      <c r="L26" s="138"/>
+      <c r="M26" s="138"/>
+      <c r="N26" s="138"/>
       <c r="O26" s="48"/>
       <c r="S26" s="1">
         <f>ROUND(MAX(0,I26-L$20*(LM!B$17+LM!B$18*'CP 1'!I26)),2)</f>
@@ -6385,8 +6386,8 @@
       </c>
     </row>
     <row r="27" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="136"/>
-      <c r="C27" s="130"/>
+      <c r="B27" s="137"/>
+      <c r="C27" s="131"/>
       <c r="D27" s="28">
         <v>22</v>
       </c>
@@ -6413,9 +6414,9 @@
         <f>IF(AND(H27&gt;=S27,H27&lt;=T27),1,0)</f>
         <v>1</v>
       </c>
-      <c r="L27" s="137"/>
-      <c r="M27" s="137"/>
-      <c r="N27" s="137"/>
+      <c r="L27" s="138"/>
+      <c r="M27" s="138"/>
+      <c r="N27" s="138"/>
       <c r="O27" s="48"/>
       <c r="S27" s="1">
         <f>ROUND(MAX(0,I27-L$20*(LM!B$17+LM!B$18*'CP 1'!I27)),2)</f>
@@ -6427,8 +6428,8 @@
       </c>
     </row>
     <row r="28" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="136"/>
-      <c r="C28" s="130"/>
+      <c r="B28" s="137"/>
+      <c r="C28" s="131"/>
       <c r="D28" s="28">
         <v>23</v>
       </c>
@@ -6455,9 +6456,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L28" s="137"/>
-      <c r="M28" s="137"/>
-      <c r="N28" s="137"/>
+      <c r="L28" s="138"/>
+      <c r="M28" s="138"/>
+      <c r="N28" s="138"/>
       <c r="O28" s="48"/>
       <c r="S28" s="1">
         <f>ROUND(MAX(0,I28-L$20*(LM!B$17+LM!B$18*'CP 1'!I28)),2)</f>
@@ -6469,8 +6470,8 @@
       </c>
     </row>
     <row r="29" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="136"/>
-      <c r="C29" s="130"/>
+      <c r="B29" s="137"/>
+      <c r="C29" s="131"/>
       <c r="D29" s="28">
         <v>24</v>
       </c>
@@ -6497,9 +6498,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L29" s="137"/>
-      <c r="M29" s="137"/>
-      <c r="N29" s="137"/>
+      <c r="L29" s="138"/>
+      <c r="M29" s="138"/>
+      <c r="N29" s="138"/>
       <c r="O29" s="48"/>
       <c r="S29" s="1">
         <f>ROUND(MAX(0,I29-L$20*(LM!B$17+LM!B$18*'CP 1'!I29)),2)</f>
@@ -6511,8 +6512,8 @@
       </c>
     </row>
     <row r="30" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="136"/>
-      <c r="C30" s="130"/>
+      <c r="B30" s="137"/>
+      <c r="C30" s="131"/>
       <c r="D30" s="28">
         <v>25</v>
       </c>
@@ -6539,9 +6540,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L30" s="137"/>
-      <c r="M30" s="137"/>
-      <c r="N30" s="137"/>
+      <c r="L30" s="138"/>
+      <c r="M30" s="138"/>
+      <c r="N30" s="138"/>
       <c r="O30" s="48"/>
       <c r="S30" s="1">
         <f>ROUND(MAX(0,I30-L$20*(LM!B$17+LM!B$18*'CP 1'!I30)),2)</f>
@@ -6553,8 +6554,8 @@
       </c>
     </row>
     <row r="31" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="136"/>
-      <c r="C31" s="130"/>
+      <c r="B31" s="137"/>
+      <c r="C31" s="131"/>
       <c r="D31" s="28">
         <v>26</v>
       </c>
@@ -6581,9 +6582,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L31" s="137"/>
-      <c r="M31" s="137"/>
-      <c r="N31" s="137"/>
+      <c r="L31" s="138"/>
+      <c r="M31" s="138"/>
+      <c r="N31" s="138"/>
       <c r="O31" s="48"/>
       <c r="S31" s="1">
         <f>ROUND(MAX(0,I31-L$20*(LM!B$17+LM!B$18*'CP 1'!I31)),2)</f>
@@ -6595,8 +6596,8 @@
       </c>
     </row>
     <row r="32" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="136"/>
-      <c r="C32" s="130"/>
+      <c r="B32" s="137"/>
+      <c r="C32" s="131"/>
       <c r="D32" s="28">
         <v>27</v>
       </c>
@@ -6623,9 +6624,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L32" s="137"/>
-      <c r="M32" s="137"/>
-      <c r="N32" s="137"/>
+      <c r="L32" s="138"/>
+      <c r="M32" s="138"/>
+      <c r="N32" s="138"/>
       <c r="O32" s="48"/>
       <c r="S32" s="1">
         <f>ROUND(MAX(0,I32-L$20*(LM!B$17+LM!B$18*'CP 1'!I32)),2)</f>
@@ -6637,8 +6638,8 @@
       </c>
     </row>
     <row r="33" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="136"/>
-      <c r="C33" s="130"/>
+      <c r="B33" s="137"/>
+      <c r="C33" s="131"/>
       <c r="D33" s="28">
         <v>28</v>
       </c>
@@ -6665,9 +6666,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L33" s="137"/>
-      <c r="M33" s="137"/>
-      <c r="N33" s="137"/>
+      <c r="L33" s="138"/>
+      <c r="M33" s="138"/>
+      <c r="N33" s="138"/>
       <c r="O33" s="48"/>
       <c r="S33" s="1">
         <f>ROUND(MAX(0,I33-L$20*(LM!B$17+LM!B$18*'CP 1'!I33)),2)</f>
@@ -6679,8 +6680,8 @@
       </c>
     </row>
     <row r="34" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="136"/>
-      <c r="C34" s="130"/>
+      <c r="B34" s="137"/>
+      <c r="C34" s="131"/>
       <c r="D34" s="28">
         <v>29</v>
       </c>
@@ -6707,9 +6708,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L34" s="137"/>
-      <c r="M34" s="137"/>
-      <c r="N34" s="137"/>
+      <c r="L34" s="138"/>
+      <c r="M34" s="138"/>
+      <c r="N34" s="138"/>
       <c r="O34" s="48"/>
       <c r="S34" s="1">
         <f>ROUND(MAX(0,I34-L$20*(LM!B$17+LM!B$18*'CP 1'!I34)),2)</f>
@@ -6721,8 +6722,8 @@
       </c>
     </row>
     <row r="35" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="136"/>
-      <c r="C35" s="130"/>
+      <c r="B35" s="137"/>
+      <c r="C35" s="131"/>
       <c r="D35" s="28">
         <v>30</v>
       </c>
@@ -6749,9 +6750,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L35" s="137"/>
-      <c r="M35" s="137"/>
-      <c r="N35" s="137"/>
+      <c r="L35" s="138"/>
+      <c r="M35" s="138"/>
+      <c r="N35" s="138"/>
       <c r="O35" s="48"/>
       <c r="S35" s="1">
         <f>ROUND(MAX(0,I35-L$20*(LM!B$17+LM!B$18*'CP 1'!I35)),2)</f>
@@ -6763,8 +6764,8 @@
       </c>
     </row>
     <row r="36" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="136"/>
-      <c r="C36" s="130"/>
+      <c r="B36" s="137"/>
+      <c r="C36" s="131"/>
       <c r="D36" s="28">
         <v>31</v>
       </c>
@@ -6791,9 +6792,9 @@
         <f>IF(AND(H36&gt;=S36,H36&lt;=T36),1,0)</f>
         <v>1</v>
       </c>
-      <c r="L36" s="137"/>
-      <c r="M36" s="137"/>
-      <c r="N36" s="137"/>
+      <c r="L36" s="138"/>
+      <c r="M36" s="138"/>
+      <c r="N36" s="138"/>
       <c r="O36" s="48"/>
       <c r="S36" s="1">
         <f>ROUND(MAX(0,I36-L$20*(LM!B$17+LM!B$18*'CP 1'!I36)),2)</f>
@@ -6805,8 +6806,8 @@
       </c>
     </row>
     <row r="37" spans="2:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="136"/>
-      <c r="C37" s="131"/>
+      <c r="B37" s="137"/>
+      <c r="C37" s="132"/>
       <c r="D37" s="30">
         <v>32</v>
       </c>
@@ -6833,9 +6834,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L37" s="137"/>
-      <c r="M37" s="137"/>
-      <c r="N37" s="137"/>
+      <c r="L37" s="138"/>
+      <c r="M37" s="138"/>
+      <c r="N37" s="138"/>
       <c r="O37" s="48"/>
       <c r="S37" s="1">
         <f>ROUND(MAX(0,I37-L$20*(LM!B$17+LM!B$18*'CP 1'!I37)),2)</f>
@@ -8624,10 +8625,10 @@
       <c r="G13" s="74">
         <v>4.83</v>
       </c>
-      <c r="K13" s="138" t="s">
+      <c r="K13" s="139" t="s">
         <v>65</v>
       </c>
-      <c r="L13" s="139"/>
+      <c r="L13" s="140"/>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C14" s="73">
@@ -8645,8 +8646,8 @@
       <c r="G14" s="74">
         <v>0</v>
       </c>
-      <c r="K14" s="140"/>
-      <c r="L14" s="141"/>
+      <c r="K14" s="141"/>
+      <c r="L14" s="142"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C15" s="73">
@@ -8664,8 +8665,8 @@
       <c r="G15" s="74">
         <v>28.8</v>
       </c>
-      <c r="K15" s="140"/>
-      <c r="L15" s="141"/>
+      <c r="K15" s="141"/>
+      <c r="L15" s="142"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C16" s="73">
@@ -8683,8 +8684,8 @@
       <c r="G16" s="74">
         <v>5.65</v>
       </c>
-      <c r="K16" s="140"/>
-      <c r="L16" s="141"/>
+      <c r="K16" s="141"/>
+      <c r="L16" s="142"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C17" s="73">
@@ -8702,8 +8703,8 @@
       <c r="G17" s="74">
         <v>0.05</v>
       </c>
-      <c r="K17" s="140"/>
-      <c r="L17" s="141"/>
+      <c r="K17" s="141"/>
+      <c r="L17" s="142"/>
     </row>
     <row r="18" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="73">
@@ -8721,8 +8722,8 @@
       <c r="G18" s="74">
         <v>3.27</v>
       </c>
-      <c r="K18" s="142"/>
-      <c r="L18" s="143"/>
+      <c r="K18" s="143"/>
+      <c r="L18" s="144"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C19" s="73">
@@ -9077,7 +9078,7 @@
       </c>
       <c r="H28" s="61">
         <f t="shared" ref="G28:H29" ca="1" si="4">RAND()</f>
-        <v>0.42510467063206758</v>
+        <v>0.64376583947533084</v>
       </c>
       <c r="N28" s="28">
         <v>7</v>
@@ -9126,7 +9127,7 @@
       </c>
       <c r="G29" s="60">
         <f t="shared" ca="1" si="4"/>
-        <v>0.14794085055857165</v>
+        <v>0.9848294406228969</v>
       </c>
       <c r="H29" s="104">
         <v>4.2099999999999999E-2</v>
@@ -9466,12 +9467,12 @@
       </c>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B37" s="157" t="s">
+      <c r="B37" s="121" t="s">
         <v>95</v>
       </c>
-      <c r="C37" s="158"/>
-      <c r="D37" s="158"/>
-      <c r="E37" s="158"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
       <c r="F37" s="55"/>
       <c r="G37" s="78" t="s">
         <v>75</v>
@@ -9506,12 +9507,12 @@
       </c>
     </row>
     <row r="38" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="159" t="s">
+      <c r="B38" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="160"/>
-      <c r="D38" s="160"/>
-      <c r="E38" s="160"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
       <c r="F38" s="45"/>
       <c r="G38" s="106" t="s">
         <v>76</v>
@@ -9591,10 +9592,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A5C9D6-2333-41E8-97C6-9FADE584365B}">
-  <dimension ref="C4:R33"/>
+  <dimension ref="C4:V33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27"/>
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9605,31 +9606,31 @@
     <col min="17" max="17" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C5" s="146" t="s">
+    <row r="4" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C5" s="145" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="147"/>
-      <c r="E5" s="147"/>
-      <c r="F5" s="147"/>
+      <c r="D5" s="146"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="146"/>
       <c r="G5" s="114" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="144" t="s">
+    <row r="6" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="147" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="145"/>
-      <c r="E6" s="145"/>
-      <c r="F6" s="145"/>
+      <c r="D6" s="148"/>
+      <c r="E6" s="148"/>
+      <c r="F6" s="148"/>
       <c r="G6" s="115" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C8" s="108" t="s">
         <v>0</v>
       </c>
@@ -9661,7 +9662,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C9" s="109">
         <v>5000</v>
       </c>
@@ -9695,7 +9696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C10" s="109">
         <v>5001</v>
       </c>
@@ -9728,8 +9729,11 @@
         <f t="shared" ref="R10:R24" si="1">IF(Q10&gt;=N10,1,0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="109">
         <v>5002</v>
       </c>
@@ -9763,7 +9767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C12" s="109">
         <v>5003</v>
       </c>
@@ -9776,11 +9780,11 @@
       <c r="F12" s="74">
         <v>747</v>
       </c>
-      <c r="I12" s="148" t="s">
+      <c r="I12" s="149" t="s">
         <v>81</v>
       </c>
-      <c r="J12" s="149"/>
-      <c r="K12" s="150"/>
+      <c r="J12" s="150"/>
+      <c r="K12" s="151"/>
       <c r="M12" s="109">
         <v>5003</v>
       </c>
@@ -9802,7 +9806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C13" s="109">
         <v>5004</v>
       </c>
@@ -9815,9 +9819,9 @@
       <c r="F13" s="74">
         <v>305</v>
       </c>
-      <c r="I13" s="151"/>
-      <c r="J13" s="152"/>
-      <c r="K13" s="153"/>
+      <c r="I13" s="152"/>
+      <c r="J13" s="153"/>
+      <c r="K13" s="154"/>
       <c r="M13" s="109">
         <v>5004</v>
       </c>
@@ -9839,7 +9843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C14" s="109">
         <v>5005</v>
       </c>
@@ -9852,9 +9856,9 @@
       <c r="F14" s="74">
         <v>770</v>
       </c>
-      <c r="I14" s="151"/>
-      <c r="J14" s="152"/>
-      <c r="K14" s="153"/>
+      <c r="I14" s="152"/>
+      <c r="J14" s="153"/>
+      <c r="K14" s="154"/>
       <c r="M14" s="109">
         <v>5005</v>
       </c>
@@ -9876,7 +9880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C15" s="109">
         <v>5006</v>
       </c>
@@ -9889,9 +9893,9 @@
       <c r="F15" s="74">
         <v>175</v>
       </c>
-      <c r="I15" s="151"/>
-      <c r="J15" s="152"/>
-      <c r="K15" s="153"/>
+      <c r="I15" s="152"/>
+      <c r="J15" s="153"/>
+      <c r="K15" s="154"/>
       <c r="M15" s="109">
         <v>5006</v>
       </c>
@@ -9913,7 +9917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="3:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="109">
         <v>5007</v>
       </c>
@@ -9926,9 +9930,9 @@
       <c r="F16" s="74">
         <v>247</v>
       </c>
-      <c r="I16" s="154"/>
-      <c r="J16" s="155"/>
-      <c r="K16" s="156"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="156"/>
+      <c r="K16" s="157"/>
       <c r="M16" s="109">
         <v>5007</v>
       </c>

</xml_diff>

<commit_message>
Bugfix, Explanation for CP and QR
</commit_message>
<xml_diff>
--- a/Analysis drafts/Miscellaneous/Approach CP und QR.xlsx
+++ b/Analysis drafts/Miscellaneous/Approach CP und QR.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Studium\Master\Université de Genève\Kurse\Master thesis\Drafts\Analysis drafts\Miscellaneous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29FA13D-D712-487D-B335-BEB8E335E9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75DAEFB-7A5F-4C28-BBBF-9A4765BE0199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{8027843B-AE8F-422B-8197-31000C3E0078}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{8027843B-AE8F-422B-8197-31000C3E0078}"/>
   </bookViews>
   <sheets>
     <sheet name="CP General" sheetId="1" r:id="rId1"/>
     <sheet name="CP 1. part" sheetId="2" r:id="rId2"/>
-    <sheet name="CP 2" sheetId="3" r:id="rId3"/>
+    <sheet name="CP 2. part" sheetId="3" r:id="rId3"/>
     <sheet name="LM" sheetId="4" r:id="rId4"/>
-    <sheet name="QR 1" sheetId="5" r:id="rId5"/>
-    <sheet name="QR 2" sheetId="6" r:id="rId6"/>
+    <sheet name="QR 1. part" sheetId="5" r:id="rId5"/>
+    <sheet name="QR 2.part" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="109">
   <si>
     <t>Id</t>
   </si>
@@ -277,10 +277,6 @@
     <t>Min</t>
   </si>
   <si>
-    <t>Prediction
-Run 1</t>
-  </si>
-  <si>
     <t>Above
 Run 1</t>
   </si>
@@ -295,34 +291,13 @@
     <t>4, 2, 1, 0.5</t>
   </si>
   <si>
-    <t>2. Make predictions with this combination and get the results</t>
-  </si>
-  <si>
-    <t>1. Provide the model every run with the whole cohort and 1 parameter combination</t>
-  </si>
-  <si>
-    <t>3. Assign the results to their respective parameter combination</t>
-  </si>
-  <si>
-    <t>4. Find the minimum deviation and select this parameter combination to produce e.g.</t>
-  </si>
-  <si>
-    <t>pnbd-model</t>
-  </si>
-  <si>
     <t>CET Upper</t>
   </si>
   <si>
     <t>CET Lower</t>
   </si>
   <si>
-    <t>1. Provide the model with the needed parameter combination to predict e.g. the lower interval boundary</t>
-  </si>
-  <si>
     <t>3. Check the coverage</t>
-  </si>
-  <si>
-    <t>(95% are desired here)</t>
   </si>
   <si>
     <t>Note</t>
@@ -338,9 +313,6 @@
   </si>
   <si>
     <t xml:space="preserve">                 for the lower boundary to avoid misleading results (not shown here)</t>
-  </si>
-  <si>
-    <t>the upper prediction interval boundaries for CET</t>
   </si>
   <si>
     <t>Parameter combination for lower boundary:</t>
@@ -410,6 +382,61 @@
 - add and subtract the result form the respective point prediction
 - check if the resulting interval covers the true value
 - calculate the overall coverage</t>
+  </si>
+  <si>
+    <t>1. Create a grid of n possible parameter combinations</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>2. Go through the grid and provide every run the whole cohort and 1 parameter combination to the model</t>
+  </si>
+  <si>
+    <t>4. Assign the results to their respective parameter combination</t>
+  </si>
+  <si>
+    <t>3. Make predictions with this combination and get the upper and lower coverage</t>
+  </si>
+  <si>
+    <t>6. Select this parameter combination to produce e.g.the upper prediction interval boundaries</t>
+  </si>
+  <si>
+    <t>5. Find the minimum deviation of the results to the desired quantile, e.g. 5% or 95%</t>
+  </si>
+  <si>
+    <t>Above
+Run 2</t>
+  </si>
+  <si>
+    <t>Below
+Run 2</t>
+  </si>
+  <si>
+    <t>Above
+Run 3</t>
+  </si>
+  <si>
+    <t>Below
+Run 3</t>
+  </si>
+  <si>
+    <t>Pred.
+Run 1</t>
+  </si>
+  <si>
+    <t>Pred.
+Run 2</t>
+  </si>
+  <si>
+    <t>Pred.
+Run 3</t>
+  </si>
+  <si>
+    <t>1. Provide the model with the needed parameter combination to predict the lower/upper interval boundary</t>
+  </si>
+  <si>
+    <t>(95% are desired here for both boundaries)</t>
   </si>
 </sst>
 </file>
@@ -992,7 +1019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1147,6 +1174,29 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1191,6 +1241,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
@@ -1255,35 +1311,25 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1478,8 +1524,8 @@
       <xdr:rowOff>181610</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2825389" cy="165366"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1572,7 +1618,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1584,7 +1630,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1596,7 +1642,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -1695,7 +1741,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1933,8 +1979,8 @@
       <xdr:rowOff>161290</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2486706" cy="157992"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -2050,7 +2096,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2062,7 +2108,7 @@
                           <a:schemeClr val="tx1"/>
                         </a:solidFill>
                         <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
@@ -2078,19 +2124,7 @@
                         <a:ea typeface="+mn-ea"/>
                         <a:cs typeface="+mn-cs"/>
                       </a:rPr>
-                      <m:t>𝒑</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="de-DE" sz="1000" b="1" i="1">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1"/>
-                        </a:solidFill>
-                        <a:effectLst/>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:rPr>
-                      <m:t>𝒓𝒆𝒅</m:t>
+                      <m:t>𝒑𝒓𝒆𝒅</m:t>
                     </m:r>
                     <m:r>
                       <a:rPr lang="de-DE" sz="1000" b="1" i="1">
@@ -2107,7 +2141,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -2407,8 +2441,8 @@
       <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3644011" cy="210507"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2604,7 +2638,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2736,8 +2770,8 @@
       <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2672270" cy="221214"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -2845,7 +2879,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -3489,10 +3523,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>462878</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>12252</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>582621</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>88452</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="422744" cy="468013"/>
     <xdr:sp macro="" textlink="">
@@ -3508,7 +3542,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4407349" y="2074134"/>
+          <a:off x="2041307" y="5008795"/>
           <a:ext cx="422744" cy="468013"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3551,10 +3585,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>544285</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>127001</xdr:rowOff>
+      <xdr:rowOff>61687</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="422744" cy="468013"/>
     <xdr:sp macro="" textlink="">
@@ -3570,7 +3604,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8658412" y="2188883"/>
+          <a:off x="4713514" y="2173516"/>
           <a:ext cx="422744" cy="468013"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3613,10 +3647,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>120649</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>108249</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>991507</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>10278</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="422744" cy="468013"/>
     <xdr:sp macro="" textlink="">
@@ -3632,7 +3666,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6239061" y="4613014"/>
+          <a:off x="10081078" y="2503107"/>
           <a:ext cx="422744" cy="468013"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3675,10 +3709,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>298823</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>44823</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>168195</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>90180</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="422744" cy="468013"/>
     <xdr:sp macro="" textlink="">
@@ -3694,7 +3728,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2136588" y="6432176"/>
+          <a:off x="5464095" y="4662180"/>
           <a:ext cx="422744" cy="468013"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3729,6 +3763,130 @@
               </a:solidFill>
             </a:rPr>
             <a:t>4.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1084410</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>33937</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="422744" cy="468013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19C1B755-8754-4D69-922A-54EAA1EB4B06}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5262710" y="6409337"/>
+          <a:ext cx="422744" cy="468013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>5.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1048658</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>116115</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="422744" cy="468013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{413B254D-BEB9-4B5A-94BC-28653DB9D495}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4299858" y="6745515"/>
+          <a:ext cx="422744" cy="468013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>6.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4468,156 +4626,6 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>54686</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38473</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1905150" cy="436786"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="TextBox 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BC5D7BF-17EE-87CB-A844-CB6CDD988A4C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6225392" y="598767"/>
-          <a:ext cx="1905150" cy="436786"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" indent="0"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Actually unknown but become</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-GB" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>visible by the time</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>600956</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>112543</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>276411</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>179295</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB390840-4222-4E18-956D-F44BAAE3A64D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7996838" y="1053837"/>
-          <a:ext cx="288044" cy="260987"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4966,23 +4974,23 @@
       <c r="G4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="156" t="s">
-        <v>93</v>
+      <c r="H4" s="120" t="s">
+        <v>84</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="120" t="s">
+      <c r="J4" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
+      <c r="K4" s="135"/>
+      <c r="L4" s="135"/>
     </row>
     <row r="5" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="128" t="s">
+      <c r="B5" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="131" t="s">
+      <c r="C5" s="146" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="2">
@@ -5003,15 +5011,15 @@
       <c r="I5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="134" t="s">
+      <c r="J5" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="134"/>
-      <c r="L5" s="134"/>
+      <c r="K5" s="149"/>
+      <c r="L5" s="149"/>
     </row>
     <row r="6" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="129"/>
-      <c r="C6" s="132"/>
+      <c r="B6" s="144"/>
+      <c r="C6" s="147"/>
       <c r="D6" s="2">
         <v>2</v>
       </c>
@@ -5030,13 +5038,13 @@
       <c r="I6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="127"/>
+      <c r="J6" s="142"/>
+      <c r="K6" s="142"/>
+      <c r="L6" s="142"/>
     </row>
     <row r="7" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="129"/>
-      <c r="C7" s="132"/>
+      <c r="B7" s="144"/>
+      <c r="C7" s="147"/>
       <c r="D7" s="2">
         <v>3</v>
       </c>
@@ -5055,13 +5063,13 @@
       <c r="I7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="127"/>
-      <c r="K7" s="127"/>
-      <c r="L7" s="127"/>
+      <c r="J7" s="142"/>
+      <c r="K7" s="142"/>
+      <c r="L7" s="142"/>
     </row>
     <row r="8" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="129"/>
-      <c r="C8" s="132"/>
+      <c r="B8" s="144"/>
+      <c r="C8" s="147"/>
       <c r="D8" s="2">
         <v>4</v>
       </c>
@@ -5080,13 +5088,13 @@
       <c r="I8" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="127"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="127"/>
+      <c r="J8" s="142"/>
+      <c r="K8" s="142"/>
+      <c r="L8" s="142"/>
     </row>
     <row r="9" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="129"/>
-      <c r="C9" s="132"/>
+      <c r="B9" s="144"/>
+      <c r="C9" s="147"/>
       <c r="D9" s="2">
         <v>5</v>
       </c>
@@ -5105,13 +5113,13 @@
       <c r="I9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="127"/>
-      <c r="K9" s="127"/>
-      <c r="L9" s="127"/>
+      <c r="J9" s="142"/>
+      <c r="K9" s="142"/>
+      <c r="L9" s="142"/>
     </row>
     <row r="10" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="129"/>
-      <c r="C10" s="132"/>
+      <c r="B10" s="144"/>
+      <c r="C10" s="147"/>
       <c r="D10" s="2">
         <v>6</v>
       </c>
@@ -5130,13 +5138,13 @@
       <c r="I10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="127"/>
-      <c r="K10" s="127"/>
-      <c r="L10" s="127"/>
+      <c r="J10" s="142"/>
+      <c r="K10" s="142"/>
+      <c r="L10" s="142"/>
     </row>
     <row r="11" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="129"/>
-      <c r="C11" s="132"/>
+      <c r="B11" s="144"/>
+      <c r="C11" s="147"/>
       <c r="D11" s="2">
         <v>7</v>
       </c>
@@ -5155,13 +5163,13 @@
       <c r="I11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="127"/>
-      <c r="K11" s="127"/>
-      <c r="L11" s="127"/>
+      <c r="J11" s="142"/>
+      <c r="K11" s="142"/>
+      <c r="L11" s="142"/>
     </row>
     <row r="12" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="129"/>
-      <c r="C12" s="132"/>
+      <c r="B12" s="144"/>
+      <c r="C12" s="147"/>
       <c r="D12" s="2">
         <v>8</v>
       </c>
@@ -5180,13 +5188,13 @@
       <c r="I12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="127"/>
-      <c r="K12" s="127"/>
-      <c r="L12" s="127"/>
+      <c r="J12" s="142"/>
+      <c r="K12" s="142"/>
+      <c r="L12" s="142"/>
     </row>
     <row r="13" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="129"/>
-      <c r="C13" s="132"/>
+      <c r="B13" s="144"/>
+      <c r="C13" s="147"/>
       <c r="D13" s="2">
         <v>9</v>
       </c>
@@ -5205,13 +5213,13 @@
       <c r="I13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="127"/>
-      <c r="K13" s="127"/>
-      <c r="L13" s="127"/>
+      <c r="J13" s="142"/>
+      <c r="K13" s="142"/>
+      <c r="L13" s="142"/>
     </row>
     <row r="14" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="129"/>
-      <c r="C14" s="132"/>
+      <c r="B14" s="144"/>
+      <c r="C14" s="147"/>
       <c r="D14" s="2">
         <v>10</v>
       </c>
@@ -5230,13 +5238,13 @@
       <c r="I14" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="127"/>
-      <c r="K14" s="127"/>
-      <c r="L14" s="127"/>
+      <c r="J14" s="142"/>
+      <c r="K14" s="142"/>
+      <c r="L14" s="142"/>
     </row>
     <row r="15" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="129"/>
-      <c r="C15" s="132"/>
+      <c r="B15" s="144"/>
+      <c r="C15" s="147"/>
       <c r="D15" s="2">
         <v>11</v>
       </c>
@@ -5255,13 +5263,13 @@
       <c r="I15" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="127"/>
-      <c r="K15" s="127"/>
-      <c r="L15" s="127"/>
+      <c r="J15" s="142"/>
+      <c r="K15" s="142"/>
+      <c r="L15" s="142"/>
     </row>
     <row r="16" spans="2:12" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="129"/>
-      <c r="C16" s="132"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="147"/>
       <c r="D16" s="2">
         <v>12</v>
       </c>
@@ -5280,13 +5288,13 @@
       <c r="I16" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="127"/>
-      <c r="K16" s="127"/>
-      <c r="L16" s="127"/>
+      <c r="J16" s="142"/>
+      <c r="K16" s="142"/>
+      <c r="L16" s="142"/>
     </row>
     <row r="17" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="129"/>
-      <c r="C17" s="133"/>
+      <c r="B17" s="144"/>
+      <c r="C17" s="148"/>
       <c r="D17" s="2">
         <v>13</v>
       </c>
@@ -5305,12 +5313,12 @@
       <c r="I17" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="127"/>
-      <c r="K17" s="127"/>
-      <c r="L17" s="127"/>
+      <c r="J17" s="142"/>
+      <c r="K17" s="142"/>
+      <c r="L17" s="142"/>
     </row>
     <row r="18" spans="2:14" s="2" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="129"/>
+      <c r="B18" s="144"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -5325,8 +5333,8 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="129"/>
-      <c r="C19" s="131" t="s">
+      <c r="B19" s="144"/>
+      <c r="C19" s="146" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="2">
@@ -5351,14 +5359,14 @@
         <f>ABS(H19-I19)</f>
         <v>1.0699999999999998</v>
       </c>
-      <c r="K19" s="127" t="s">
+      <c r="K19" s="142" t="s">
         <v>13</v>
       </c>
-      <c r="L19" s="127"/>
+      <c r="L19" s="142"/>
     </row>
     <row r="20" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="129"/>
-      <c r="C20" s="132"/>
+      <c r="B20" s="144"/>
+      <c r="C20" s="147"/>
       <c r="D20" s="2">
         <v>15</v>
       </c>
@@ -5381,12 +5389,12 @@
         <f t="shared" ref="J20:J30" si="0">ABS(H20-I20)</f>
         <v>1.5700000000000003</v>
       </c>
-      <c r="K20" s="127"/>
-      <c r="L20" s="127"/>
+      <c r="K20" s="142"/>
+      <c r="L20" s="142"/>
     </row>
     <row r="21" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="129"/>
-      <c r="C21" s="132"/>
+      <c r="B21" s="144"/>
+      <c r="C21" s="147"/>
       <c r="D21" s="2">
         <v>16</v>
       </c>
@@ -5409,12 +5417,12 @@
         <f t="shared" si="0"/>
         <v>23.58</v>
       </c>
-      <c r="K21" s="127"/>
-      <c r="L21" s="127"/>
+      <c r="K21" s="142"/>
+      <c r="L21" s="142"/>
     </row>
     <row r="22" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="129"/>
-      <c r="C22" s="132"/>
+      <c r="B22" s="144"/>
+      <c r="C22" s="147"/>
       <c r="D22" s="2">
         <v>17</v>
       </c>
@@ -5437,12 +5445,12 @@
         <f t="shared" si="0"/>
         <v>4.25</v>
       </c>
-      <c r="K22" s="127"/>
-      <c r="L22" s="127"/>
+      <c r="K22" s="142"/>
+      <c r="L22" s="142"/>
     </row>
     <row r="23" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="129"/>
-      <c r="C23" s="132"/>
+      <c r="B23" s="144"/>
+      <c r="C23" s="147"/>
       <c r="D23" s="2">
         <v>18</v>
       </c>
@@ -5465,12 +5473,12 @@
         <f t="shared" si="0"/>
         <v>0.43</v>
       </c>
-      <c r="K23" s="127"/>
-      <c r="L23" s="127"/>
+      <c r="K23" s="142"/>
+      <c r="L23" s="142"/>
     </row>
     <row r="24" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="129"/>
-      <c r="C24" s="132"/>
+      <c r="B24" s="144"/>
+      <c r="C24" s="147"/>
       <c r="D24" s="2">
         <v>19</v>
       </c>
@@ -5493,12 +5501,12 @@
         <f t="shared" si="0"/>
         <v>3.95</v>
       </c>
-      <c r="K24" s="127"/>
-      <c r="L24" s="127"/>
+      <c r="K24" s="142"/>
+      <c r="L24" s="142"/>
     </row>
     <row r="25" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="129"/>
-      <c r="C25" s="132"/>
+      <c r="B25" s="144"/>
+      <c r="C25" s="147"/>
       <c r="D25" s="2">
         <v>20</v>
       </c>
@@ -5521,12 +5529,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="K25" s="127"/>
-      <c r="L25" s="127"/>
+      <c r="K25" s="142"/>
+      <c r="L25" s="142"/>
     </row>
     <row r="26" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="129"/>
-      <c r="C26" s="132"/>
+      <c r="B26" s="144"/>
+      <c r="C26" s="147"/>
       <c r="D26" s="2">
         <v>21</v>
       </c>
@@ -5549,12 +5557,12 @@
         <f t="shared" si="0"/>
         <v>8.9999999999999858E-2</v>
       </c>
-      <c r="K26" s="127"/>
-      <c r="L26" s="127"/>
+      <c r="K26" s="142"/>
+      <c r="L26" s="142"/>
     </row>
     <row r="27" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="129"/>
-      <c r="C27" s="132"/>
+      <c r="B27" s="144"/>
+      <c r="C27" s="147"/>
       <c r="D27" s="2">
         <v>22</v>
       </c>
@@ -5577,12 +5585,12 @@
         <f t="shared" si="0"/>
         <v>9.9799999999999986</v>
       </c>
-      <c r="K27" s="127"/>
-      <c r="L27" s="127"/>
+      <c r="K27" s="142"/>
+      <c r="L27" s="142"/>
     </row>
     <row r="28" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="129"/>
-      <c r="C28" s="132"/>
+      <c r="B28" s="144"/>
+      <c r="C28" s="147"/>
       <c r="D28" s="2">
         <v>23</v>
       </c>
@@ -5605,12 +5613,12 @@
         <f t="shared" si="0"/>
         <v>2.3899999999999997</v>
       </c>
-      <c r="K28" s="127"/>
-      <c r="L28" s="127"/>
+      <c r="K28" s="142"/>
+      <c r="L28" s="142"/>
     </row>
     <row r="29" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="129"/>
-      <c r="C29" s="132"/>
+      <c r="B29" s="144"/>
+      <c r="C29" s="147"/>
       <c r="D29" s="2">
         <v>24</v>
       </c>
@@ -5633,12 +5641,12 @@
         <f t="shared" si="0"/>
         <v>15.59</v>
       </c>
-      <c r="K29" s="127"/>
-      <c r="L29" s="127"/>
+      <c r="K29" s="142"/>
+      <c r="L29" s="142"/>
     </row>
     <row r="30" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="130"/>
-      <c r="C30" s="133"/>
+      <c r="B30" s="145"/>
+      <c r="C30" s="148"/>
       <c r="D30" s="2">
         <v>25</v>
       </c>
@@ -5661,9 +5669,9 @@
         <f t="shared" si="0"/>
         <v>0.04</v>
       </c>
-      <c r="K30" s="127"/>
-      <c r="L30" s="127"/>
-      <c r="M30" s="157">
+      <c r="K30" s="142"/>
+      <c r="L30" s="142"/>
+      <c r="M30" s="121">
         <f>_xlfn.PERCENTILE.INC(J19:J30,0.9)</f>
         <v>15.029000000000002</v>
       </c>
@@ -5686,10 +5694,10 @@
       <c r="L31" s="4"/>
     </row>
     <row r="32" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="121" t="s">
+      <c r="B32" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="122"/>
+      <c r="C32" s="137"/>
       <c r="D32" s="2">
         <v>26</v>
       </c>
@@ -5709,21 +5717,21 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="J32" s="21" t="str">
-        <f>_xlfn.CONCAT("[",I32-M$30,", ",I32+M$30,"]")</f>
+        <f t="shared" ref="J32:J38" si="1">_xlfn.CONCAT("[",I32-M$30,", ",I32+M$30,"]")</f>
         <v>[-14.749, 15.309]</v>
       </c>
       <c r="K32" s="2">
         <v>1</v>
       </c>
-      <c r="L32" s="127" t="s">
-        <v>95</v>
-      </c>
-      <c r="M32" s="127"/>
-      <c r="N32" s="127"/>
+      <c r="L32" s="142" t="s">
+        <v>86</v>
+      </c>
+      <c r="M32" s="142"/>
+      <c r="N32" s="142"/>
     </row>
     <row r="33" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="123"/>
-      <c r="C33" s="124"/>
+      <c r="B33" s="138"/>
+      <c r="C33" s="139"/>
       <c r="D33" s="2">
         <v>27</v>
       </c>
@@ -5743,19 +5751,19 @@
         <v>16.649999999999999</v>
       </c>
       <c r="J33" s="21" t="str">
-        <f>_xlfn.CONCAT("[",I33-M$30,", ",I33+M$30,"]")</f>
+        <f t="shared" si="1"/>
         <v>[1.621, 31.679]</v>
       </c>
       <c r="K33" s="2">
         <v>0</v>
       </c>
-      <c r="L33" s="127"/>
-      <c r="M33" s="127"/>
-      <c r="N33" s="127"/>
+      <c r="L33" s="142"/>
+      <c r="M33" s="142"/>
+      <c r="N33" s="142"/>
     </row>
     <row r="34" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="123"/>
-      <c r="C34" s="124"/>
+      <c r="B34" s="138"/>
+      <c r="C34" s="139"/>
       <c r="D34" s="2">
         <v>28</v>
       </c>
@@ -5775,19 +5783,19 @@
         <v>1.38</v>
       </c>
       <c r="J34" s="21" t="str">
-        <f>_xlfn.CONCAT("[",I34-M$30,", ",I34+M$30,"]")</f>
+        <f t="shared" si="1"/>
         <v>[-13.649, 16.409]</v>
       </c>
       <c r="K34" s="2">
         <v>1</v>
       </c>
-      <c r="L34" s="127"/>
-      <c r="M34" s="127"/>
-      <c r="N34" s="127"/>
+      <c r="L34" s="142"/>
+      <c r="M34" s="142"/>
+      <c r="N34" s="142"/>
     </row>
     <row r="35" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="123"/>
-      <c r="C35" s="124"/>
+      <c r="B35" s="138"/>
+      <c r="C35" s="139"/>
       <c r="D35" s="2">
         <v>29</v>
       </c>
@@ -5807,19 +5815,19 @@
         <v>10.8</v>
       </c>
       <c r="J35" s="21" t="str">
-        <f>_xlfn.CONCAT("[",I35-M$30,", ",I35+M$30,"]")</f>
+        <f t="shared" si="1"/>
         <v>[-4.229, 25.829]</v>
       </c>
       <c r="K35" s="2">
         <v>1</v>
       </c>
-      <c r="L35" s="127"/>
-      <c r="M35" s="127"/>
-      <c r="N35" s="127"/>
+      <c r="L35" s="142"/>
+      <c r="M35" s="142"/>
+      <c r="N35" s="142"/>
     </row>
     <row r="36" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="123"/>
-      <c r="C36" s="124"/>
+      <c r="B36" s="138"/>
+      <c r="C36" s="139"/>
       <c r="D36" s="2">
         <v>30</v>
       </c>
@@ -5839,19 +5847,19 @@
         <v>5.22</v>
       </c>
       <c r="J36" s="21" t="str">
-        <f>_xlfn.CONCAT("[",I36-M$30,", ",I36+M$30,"]")</f>
+        <f t="shared" si="1"/>
         <v>[-9.809, 20.249]</v>
       </c>
       <c r="K36" s="2">
         <v>1</v>
       </c>
-      <c r="L36" s="127"/>
-      <c r="M36" s="127"/>
-      <c r="N36" s="127"/>
+      <c r="L36" s="142"/>
+      <c r="M36" s="142"/>
+      <c r="N36" s="142"/>
     </row>
     <row r="37" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="123"/>
-      <c r="C37" s="124"/>
+      <c r="B37" s="138"/>
+      <c r="C37" s="139"/>
       <c r="D37" s="2">
         <v>31</v>
       </c>
@@ -5871,19 +5879,19 @@
         <v>28.5</v>
       </c>
       <c r="J37" s="21" t="str">
-        <f>_xlfn.CONCAT("[",I37-M$30,", ",I37+M$30,"]")</f>
+        <f t="shared" si="1"/>
         <v>[13.471, 43.529]</v>
       </c>
       <c r="K37" s="2">
         <v>0</v>
       </c>
-      <c r="L37" s="127"/>
-      <c r="M37" s="127"/>
-      <c r="N37" s="127"/>
+      <c r="L37" s="142"/>
+      <c r="M37" s="142"/>
+      <c r="N37" s="142"/>
     </row>
     <row r="38" spans="2:14" s="2" customFormat="1" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="125"/>
-      <c r="C38" s="126"/>
+      <c r="B38" s="140"/>
+      <c r="C38" s="141"/>
       <c r="D38" s="2">
         <v>32</v>
       </c>
@@ -5902,20 +5910,20 @@
       <c r="I38" s="18">
         <v>0</v>
       </c>
-      <c r="J38" s="158" t="str">
-        <f>_xlfn.CONCAT("[",I38-M$30,", ",I38+M$30,"]")</f>
+      <c r="J38" s="122" t="str">
+        <f t="shared" si="1"/>
         <v>[-15.029, 15.029]</v>
       </c>
-      <c r="K38" s="159">
-        <v>1</v>
-      </c>
-      <c r="L38" s="127"/>
-      <c r="M38" s="127"/>
-      <c r="N38" s="127"/>
+      <c r="K38" s="123">
+        <v>1</v>
+      </c>
+      <c r="L38" s="142"/>
+      <c r="M38" s="142"/>
+      <c r="N38" s="142"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="J39" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="K39">
         <f>ROUND(AVERAGE(K32:K38),2)</f>
@@ -5975,11 +5983,11 @@
       <c r="G4" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="160" t="s">
-        <v>93</v>
+      <c r="H4" s="124" t="s">
+        <v>84</v>
       </c>
       <c r="I4" s="42" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J4" s="25" t="s">
         <v>15</v>
@@ -5989,10 +5997,10 @@
       </c>
     </row>
     <row r="5" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="135" t="s">
+      <c r="B5" s="152" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="128" t="s">
+      <c r="C5" s="143" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="26">
@@ -6021,14 +6029,14 @@
         <f>ROUND(J5/(LM!B$17+LM!B$18*'CP 1. part'!I5),2)</f>
         <v>0.8</v>
       </c>
-      <c r="L5" s="136" t="s">
-        <v>97</v>
-      </c>
-      <c r="M5" s="136"/>
+      <c r="L5" s="153" t="s">
+        <v>88</v>
+      </c>
+      <c r="M5" s="153"/>
     </row>
     <row r="6" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="135"/>
-      <c r="C6" s="129"/>
+      <c r="B6" s="152"/>
+      <c r="C6" s="144"/>
       <c r="D6" s="28">
         <v>2</v>
       </c>
@@ -6055,12 +6063,12 @@
         <f>ROUND(J6/(LM!B$17+LM!B$18*'CP 1. part'!I6),2)</f>
         <v>1.03</v>
       </c>
-      <c r="L6" s="136"/>
-      <c r="M6" s="136"/>
+      <c r="L6" s="153"/>
+      <c r="M6" s="153"/>
     </row>
     <row r="7" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="135"/>
-      <c r="C7" s="129"/>
+      <c r="B7" s="152"/>
+      <c r="C7" s="144"/>
       <c r="D7" s="28">
         <v>3</v>
       </c>
@@ -6087,12 +6095,12 @@
         <f>ROUND(J7/(LM!B$17+LM!B$18*'CP 1. part'!I7),2)</f>
         <v>0.67</v>
       </c>
-      <c r="L7" s="136"/>
-      <c r="M7" s="136"/>
+      <c r="L7" s="153"/>
+      <c r="M7" s="153"/>
     </row>
     <row r="8" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="135"/>
-      <c r="C8" s="129"/>
+      <c r="B8" s="152"/>
+      <c r="C8" s="144"/>
       <c r="D8" s="28">
         <v>4</v>
       </c>
@@ -6119,16 +6127,16 @@
         <f>ROUND(J8/(LM!B$17+LM!B$18*'CP 1. part'!I8),2)</f>
         <v>0.12</v>
       </c>
-      <c r="L8" s="136"/>
-      <c r="M8" s="136"/>
-      <c r="O8" s="170" t="s">
-        <v>96</v>
-      </c>
-      <c r="P8" s="170"/>
+      <c r="L8" s="153"/>
+      <c r="M8" s="153"/>
+      <c r="O8" s="150" t="s">
+        <v>87</v>
+      </c>
+      <c r="P8" s="150"/>
     </row>
     <row r="9" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="135"/>
-      <c r="C9" s="129"/>
+      <c r="B9" s="152"/>
+      <c r="C9" s="144"/>
       <c r="D9" s="28">
         <v>5</v>
       </c>
@@ -6155,14 +6163,14 @@
         <f>ROUND(J9/(LM!B$17+LM!B$18*'CP 1. part'!I9),2)</f>
         <v>0.2</v>
       </c>
-      <c r="L9" s="136"/>
-      <c r="M9" s="136"/>
-      <c r="O9" s="171"/>
-      <c r="P9" s="171"/>
+      <c r="L9" s="153"/>
+      <c r="M9" s="153"/>
+      <c r="O9" s="151"/>
+      <c r="P9" s="151"/>
     </row>
     <row r="10" spans="2:17" s="1" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="135"/>
-      <c r="C10" s="129"/>
+      <c r="B10" s="152"/>
+      <c r="C10" s="144"/>
       <c r="D10" s="28">
         <v>6</v>
       </c>
@@ -6189,16 +6197,16 @@
         <f>ROUND(J10/(LM!B$17+LM!B$18*'CP 1. part'!I10),2)</f>
         <v>1.1399999999999999</v>
       </c>
-      <c r="L10" s="136"/>
-      <c r="M10" s="136"/>
-      <c r="O10" s="161" t="s">
+      <c r="L10" s="153"/>
+      <c r="M10" s="153"/>
+      <c r="O10" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="P10" s="162"/>
+      <c r="P10" s="126"/>
     </row>
     <row r="11" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="135"/>
-      <c r="C11" s="129"/>
+      <c r="B11" s="152"/>
+      <c r="C11" s="144"/>
       <c r="D11" s="28">
         <v>7</v>
       </c>
@@ -6225,18 +6233,18 @@
         <f>ROUND(J11/(LM!B$17+LM!B$18*'CP 1. part'!I11),2)</f>
         <v>0.33</v>
       </c>
-      <c r="L11" s="136"/>
-      <c r="M11" s="136"/>
-      <c r="O11" s="163" t="s">
+      <c r="L11" s="153"/>
+      <c r="M11" s="153"/>
+      <c r="O11" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="P11" s="164">
+      <c r="P11" s="128">
         <v>1.07</v>
       </c>
     </row>
     <row r="12" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="135"/>
-      <c r="C12" s="129"/>
+      <c r="B12" s="152"/>
+      <c r="C12" s="144"/>
       <c r="D12" s="28">
         <v>8</v>
       </c>
@@ -6263,8 +6271,8 @@
         <f>ROUND(J12/(LM!B$17+LM!B$18*'CP 1. part'!I12),2)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="L12" s="136"/>
-      <c r="M12" s="136"/>
+      <c r="L12" s="153"/>
+      <c r="M12" s="153"/>
       <c r="O12" s="71" t="s">
         <v>18</v>
       </c>
@@ -6273,8 +6281,8 @@
       </c>
     </row>
     <row r="13" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="135"/>
-      <c r="C13" s="129"/>
+      <c r="B13" s="152"/>
+      <c r="C13" s="144"/>
       <c r="D13" s="28">
         <v>9</v>
       </c>
@@ -6301,8 +6309,8 @@
         <f>ROUND(J13/(LM!B$17+LM!B$18*'CP 1. part'!I13),2)</f>
         <v>0.03</v>
       </c>
-      <c r="L13" s="136"/>
-      <c r="M13" s="136"/>
+      <c r="L13" s="153"/>
+      <c r="M13" s="153"/>
       <c r="O13" s="71" t="s">
         <v>19</v>
       </c>
@@ -6311,8 +6319,8 @@
       </c>
     </row>
     <row r="14" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="135"/>
-      <c r="C14" s="129"/>
+      <c r="B14" s="152"/>
+      <c r="C14" s="144"/>
       <c r="D14" s="28">
         <v>10</v>
       </c>
@@ -6339,18 +6347,18 @@
         <f>ROUND(J14/(LM!B$17+LM!B$18*'CP 1. part'!I14),2)</f>
         <v>0.69</v>
       </c>
-      <c r="L14" s="136"/>
-      <c r="M14" s="136"/>
+      <c r="L14" s="153"/>
+      <c r="M14" s="153"/>
       <c r="O14" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="P14" s="165" t="s">
+      <c r="P14" s="129" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="135"/>
-      <c r="C15" s="129"/>
+      <c r="B15" s="152"/>
+      <c r="C15" s="144"/>
       <c r="D15" s="28">
         <v>11</v>
       </c>
@@ -6377,18 +6385,18 @@
         <f>ROUND(J15/(LM!B$17+LM!B$18*'CP 1. part'!I15),2)</f>
         <v>0.95</v>
       </c>
-      <c r="L15" s="136"/>
-      <c r="M15" s="136"/>
+      <c r="L15" s="153"/>
+      <c r="M15" s="153"/>
       <c r="O15" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="P15" s="165" t="s">
+      <c r="P15" s="129" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:17" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="135"/>
-      <c r="C16" s="129"/>
+      <c r="B16" s="152"/>
+      <c r="C16" s="144"/>
       <c r="D16" s="28">
         <v>12</v>
       </c>
@@ -6415,18 +6423,18 @@
         <f>ROUND(J16/(LM!B$17+LM!B$18*'CP 1. part'!I16),2)</f>
         <v>0.56999999999999995</v>
       </c>
-      <c r="L16" s="136"/>
-      <c r="M16" s="136"/>
+      <c r="L16" s="153"/>
+      <c r="M16" s="153"/>
       <c r="O16" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="P16" s="165" t="s">
+      <c r="P16" s="129" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="135"/>
-      <c r="C17" s="129"/>
+      <c r="B17" s="152"/>
+      <c r="C17" s="144"/>
       <c r="D17" s="28">
         <v>13</v>
       </c>
@@ -6453,18 +6461,18 @@
         <f>ROUND(J17/(LM!B$17+LM!B$18*'CP 1. part'!I17),2)</f>
         <v>0.83</v>
       </c>
-      <c r="L17" s="136"/>
-      <c r="M17" s="136"/>
+      <c r="L17" s="153"/>
+      <c r="M17" s="153"/>
       <c r="O17" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="P17" s="165" t="s">
+      <c r="P17" s="129" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="135"/>
-      <c r="C18" s="129"/>
+      <c r="B18" s="152"/>
+      <c r="C18" s="144"/>
       <c r="D18" s="28">
         <v>14</v>
       </c>
@@ -6491,18 +6499,18 @@
         <f>ROUND(J18/(LM!B$17+LM!B$18*'CP 1. part'!I18),2)</f>
         <v>0.56999999999999995</v>
       </c>
-      <c r="L18" s="136"/>
-      <c r="M18" s="136"/>
-      <c r="O18" s="166" t="s">
-        <v>99</v>
-      </c>
-      <c r="P18" s="167">
+      <c r="L18" s="153"/>
+      <c r="M18" s="153"/>
+      <c r="O18" s="130" t="s">
+        <v>90</v>
+      </c>
+      <c r="P18" s="131">
         <v>1.59</v>
       </c>
     </row>
     <row r="19" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="135"/>
-      <c r="C19" s="129"/>
+      <c r="B19" s="152"/>
+      <c r="C19" s="144"/>
       <c r="D19" s="28">
         <v>15</v>
       </c>
@@ -6529,14 +6537,14 @@
         <f>ROUND(J19/(LM!B$17+LM!B$18*'CP 1. part'!I19),2)</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="L19" s="136"/>
-      <c r="M19" s="136"/>
-      <c r="O19" s="168"/>
+      <c r="L19" s="153"/>
+      <c r="M19" s="153"/>
+      <c r="O19" s="132"/>
       <c r="P19" s="72"/>
     </row>
     <row r="20" spans="2:20" s="1" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="135"/>
-      <c r="C20" s="130"/>
+      <c r="B20" s="152"/>
+      <c r="C20" s="145"/>
       <c r="D20" s="30">
         <v>16</v>
       </c>
@@ -6568,7 +6576,7 @@
         <v>1.07</v>
       </c>
       <c r="M20" s="24"/>
-      <c r="O20" s="169" t="s">
+      <c r="O20" s="133" t="s">
         <v>21</v>
       </c>
       <c r="P20" s="104">
@@ -6576,7 +6584,7 @@
       </c>
     </row>
     <row r="21" spans="2:20" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="135"/>
+      <c r="B21" s="152"/>
       <c r="I21" s="33"/>
       <c r="J21" s="51" t="s">
         <v>10</v>
@@ -6592,8 +6600,8 @@
       </c>
     </row>
     <row r="22" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="135"/>
-      <c r="C22" s="128" t="s">
+      <c r="B22" s="152"/>
+      <c r="C22" s="143" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="26">
@@ -6622,11 +6630,11 @@
         <f>IF(AND(H22&gt;=S22,H22&lt;=T22),1,0)</f>
         <v>0</v>
       </c>
-      <c r="L22" s="136" t="s">
-        <v>98</v>
-      </c>
-      <c r="M22" s="136"/>
-      <c r="N22" s="136"/>
+      <c r="L22" s="153" t="s">
+        <v>89</v>
+      </c>
+      <c r="M22" s="153"/>
+      <c r="N22" s="153"/>
       <c r="O22" s="46"/>
       <c r="S22" s="1">
         <f>ROUND(MAX(0,I22-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I22)),2)</f>
@@ -6638,8 +6646,8 @@
       </c>
     </row>
     <row r="23" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="135"/>
-      <c r="C23" s="129"/>
+      <c r="B23" s="152"/>
+      <c r="C23" s="144"/>
       <c r="D23" s="28">
         <v>18</v>
       </c>
@@ -6663,12 +6671,12 @@
         <v>[0, 2.85]</v>
       </c>
       <c r="K23" s="35">
-        <f t="shared" ref="K22:K37" si="1">IF(AND(H23&gt;=S23,H23&lt;=T23),1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="L23" s="136"/>
-      <c r="M23" s="136"/>
-      <c r="N23" s="136"/>
+        <f t="shared" ref="K23:K37" si="1">IF(AND(H23&gt;=S23,H23&lt;=T23),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L23" s="153"/>
+      <c r="M23" s="153"/>
+      <c r="N23" s="153"/>
       <c r="O23" s="46"/>
       <c r="S23" s="1">
         <f>ROUND(MAX(0,I23-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I23)),2)</f>
@@ -6680,8 +6688,8 @@
       </c>
     </row>
     <row r="24" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="135"/>
-      <c r="C24" s="129"/>
+      <c r="B24" s="152"/>
+      <c r="C24" s="144"/>
       <c r="D24" s="28">
         <v>19</v>
       </c>
@@ -6708,9 +6716,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L24" s="136"/>
-      <c r="M24" s="136"/>
-      <c r="N24" s="136"/>
+      <c r="L24" s="153"/>
+      <c r="M24" s="153"/>
+      <c r="N24" s="153"/>
       <c r="O24" s="46"/>
       <c r="S24" s="1">
         <f>ROUND(MAX(0,I24-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I24)),2)</f>
@@ -6722,8 +6730,8 @@
       </c>
     </row>
     <row r="25" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="135"/>
-      <c r="C25" s="129"/>
+      <c r="B25" s="152"/>
+      <c r="C25" s="144"/>
       <c r="D25" s="28">
         <v>20</v>
       </c>
@@ -6750,9 +6758,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L25" s="136"/>
-      <c r="M25" s="136"/>
-      <c r="N25" s="136"/>
+      <c r="L25" s="153"/>
+      <c r="M25" s="153"/>
+      <c r="N25" s="153"/>
       <c r="O25" s="46"/>
       <c r="S25" s="1">
         <f>ROUND(MAX(0,I25-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I25)),2)</f>
@@ -6764,8 +6772,8 @@
       </c>
     </row>
     <row r="26" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="135"/>
-      <c r="C26" s="129"/>
+      <c r="B26" s="152"/>
+      <c r="C26" s="144"/>
       <c r="D26" s="28">
         <v>21</v>
       </c>
@@ -6792,9 +6800,9 @@
         <f>IF(AND(H26&gt;=S26,H26&lt;=T26),1,0)</f>
         <v>0</v>
       </c>
-      <c r="L26" s="136"/>
-      <c r="M26" s="136"/>
-      <c r="N26" s="136"/>
+      <c r="L26" s="153"/>
+      <c r="M26" s="153"/>
+      <c r="N26" s="153"/>
       <c r="O26" s="46"/>
       <c r="S26" s="1">
         <f>ROUND(MAX(0,I26-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I26)),2)</f>
@@ -6806,8 +6814,8 @@
       </c>
     </row>
     <row r="27" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="135"/>
-      <c r="C27" s="129"/>
+      <c r="B27" s="152"/>
+      <c r="C27" s="144"/>
       <c r="D27" s="28">
         <v>22</v>
       </c>
@@ -6834,9 +6842,9 @@
         <f>IF(AND(H27&gt;=S27,H27&lt;=T27),1,0)</f>
         <v>1</v>
       </c>
-      <c r="L27" s="136"/>
-      <c r="M27" s="136"/>
-      <c r="N27" s="136"/>
+      <c r="L27" s="153"/>
+      <c r="M27" s="153"/>
+      <c r="N27" s="153"/>
       <c r="O27" s="46"/>
       <c r="S27" s="1">
         <f>ROUND(MAX(0,I27-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I27)),2)</f>
@@ -6848,8 +6856,8 @@
       </c>
     </row>
     <row r="28" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="135"/>
-      <c r="C28" s="129"/>
+      <c r="B28" s="152"/>
+      <c r="C28" s="144"/>
       <c r="D28" s="28">
         <v>23</v>
       </c>
@@ -6876,9 +6884,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L28" s="136"/>
-      <c r="M28" s="136"/>
-      <c r="N28" s="136"/>
+      <c r="L28" s="153"/>
+      <c r="M28" s="153"/>
+      <c r="N28" s="153"/>
       <c r="O28" s="46"/>
       <c r="S28" s="1">
         <f>ROUND(MAX(0,I28-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I28)),2)</f>
@@ -6890,8 +6898,8 @@
       </c>
     </row>
     <row r="29" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="135"/>
-      <c r="C29" s="129"/>
+      <c r="B29" s="152"/>
+      <c r="C29" s="144"/>
       <c r="D29" s="28">
         <v>24</v>
       </c>
@@ -6918,9 +6926,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L29" s="136"/>
-      <c r="M29" s="136"/>
-      <c r="N29" s="136"/>
+      <c r="L29" s="153"/>
+      <c r="M29" s="153"/>
+      <c r="N29" s="153"/>
       <c r="O29" s="46"/>
       <c r="S29" s="1">
         <f>ROUND(MAX(0,I29-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I29)),2)</f>
@@ -6932,8 +6940,8 @@
       </c>
     </row>
     <row r="30" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="135"/>
-      <c r="C30" s="129"/>
+      <c r="B30" s="152"/>
+      <c r="C30" s="144"/>
       <c r="D30" s="28">
         <v>25</v>
       </c>
@@ -6960,9 +6968,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L30" s="136"/>
-      <c r="M30" s="136"/>
-      <c r="N30" s="136"/>
+      <c r="L30" s="153"/>
+      <c r="M30" s="153"/>
+      <c r="N30" s="153"/>
       <c r="O30" s="46"/>
       <c r="S30" s="1">
         <f>ROUND(MAX(0,I30-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I30)),2)</f>
@@ -6974,8 +6982,8 @@
       </c>
     </row>
     <row r="31" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="135"/>
-      <c r="C31" s="129"/>
+      <c r="B31" s="152"/>
+      <c r="C31" s="144"/>
       <c r="D31" s="28">
         <v>26</v>
       </c>
@@ -7002,9 +7010,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L31" s="136"/>
-      <c r="M31" s="136"/>
-      <c r="N31" s="136"/>
+      <c r="L31" s="153"/>
+      <c r="M31" s="153"/>
+      <c r="N31" s="153"/>
       <c r="O31" s="46"/>
       <c r="S31" s="1">
         <f>ROUND(MAX(0,I31-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I31)),2)</f>
@@ -7016,8 +7024,8 @@
       </c>
     </row>
     <row r="32" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="135"/>
-      <c r="C32" s="129"/>
+      <c r="B32" s="152"/>
+      <c r="C32" s="144"/>
       <c r="D32" s="28">
         <v>27</v>
       </c>
@@ -7044,9 +7052,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L32" s="136"/>
-      <c r="M32" s="136"/>
-      <c r="N32" s="136"/>
+      <c r="L32" s="153"/>
+      <c r="M32" s="153"/>
+      <c r="N32" s="153"/>
       <c r="O32" s="46"/>
       <c r="S32" s="1">
         <f>ROUND(MAX(0,I32-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I32)),2)</f>
@@ -7058,8 +7066,8 @@
       </c>
     </row>
     <row r="33" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="135"/>
-      <c r="C33" s="129"/>
+      <c r="B33" s="152"/>
+      <c r="C33" s="144"/>
       <c r="D33" s="28">
         <v>28</v>
       </c>
@@ -7086,9 +7094,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L33" s="136"/>
-      <c r="M33" s="136"/>
-      <c r="N33" s="136"/>
+      <c r="L33" s="153"/>
+      <c r="M33" s="153"/>
+      <c r="N33" s="153"/>
       <c r="O33" s="46"/>
       <c r="S33" s="1">
         <f>ROUND(MAX(0,I33-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I33)),2)</f>
@@ -7100,8 +7108,8 @@
       </c>
     </row>
     <row r="34" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="135"/>
-      <c r="C34" s="129"/>
+      <c r="B34" s="152"/>
+      <c r="C34" s="144"/>
       <c r="D34" s="28">
         <v>29</v>
       </c>
@@ -7128,9 +7136,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L34" s="136"/>
-      <c r="M34" s="136"/>
-      <c r="N34" s="136"/>
+      <c r="L34" s="153"/>
+      <c r="M34" s="153"/>
+      <c r="N34" s="153"/>
       <c r="O34" s="46"/>
       <c r="S34" s="1">
         <f>ROUND(MAX(0,I34-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I34)),2)</f>
@@ -7142,8 +7150,8 @@
       </c>
     </row>
     <row r="35" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="135"/>
-      <c r="C35" s="129"/>
+      <c r="B35" s="152"/>
+      <c r="C35" s="144"/>
       <c r="D35" s="28">
         <v>30</v>
       </c>
@@ -7170,9 +7178,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L35" s="136"/>
-      <c r="M35" s="136"/>
-      <c r="N35" s="136"/>
+      <c r="L35" s="153"/>
+      <c r="M35" s="153"/>
+      <c r="N35" s="153"/>
       <c r="O35" s="46"/>
       <c r="S35" s="1">
         <f>ROUND(MAX(0,I35-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I35)),2)</f>
@@ -7184,8 +7192,8 @@
       </c>
     </row>
     <row r="36" spans="2:20" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="135"/>
-      <c r="C36" s="129"/>
+      <c r="B36" s="152"/>
+      <c r="C36" s="144"/>
       <c r="D36" s="28">
         <v>31</v>
       </c>
@@ -7212,9 +7220,9 @@
         <f>IF(AND(H36&gt;=S36,H36&lt;=T36),1,0)</f>
         <v>1</v>
       </c>
-      <c r="L36" s="136"/>
-      <c r="M36" s="136"/>
-      <c r="N36" s="136"/>
+      <c r="L36" s="153"/>
+      <c r="M36" s="153"/>
+      <c r="N36" s="153"/>
       <c r="O36" s="46"/>
       <c r="S36" s="1">
         <f>ROUND(MAX(0,I36-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I36)),2)</f>
@@ -7226,8 +7234,8 @@
       </c>
     </row>
     <row r="37" spans="2:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="135"/>
-      <c r="C37" s="130"/>
+      <c r="B37" s="152"/>
+      <c r="C37" s="145"/>
       <c r="D37" s="30">
         <v>32</v>
       </c>
@@ -7254,9 +7262,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L37" s="136"/>
-      <c r="M37" s="136"/>
-      <c r="N37" s="136"/>
+      <c r="L37" s="153"/>
+      <c r="M37" s="153"/>
+      <c r="N37" s="153"/>
       <c r="O37" s="46"/>
       <c r="S37" s="1">
         <f>ROUND(MAX(0,I37-L$20*(LM!B$17+LM!B$18*'CP 1. part'!I37)),2)</f>
@@ -7291,8 +7299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9750A8F5-A2B1-4E18-9C47-5331C8CFD2B2}">
   <dimension ref="C3:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7317,11 +7325,11 @@
       <c r="F4" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="172" t="s">
-        <v>93</v>
+      <c r="G4" s="134" t="s">
+        <v>84</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="I4" s="50" t="s">
         <v>51</v>
@@ -7457,12 +7465,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M7" s="136" t="s">
-        <v>101</v>
-      </c>
-      <c r="N7" s="136"/>
-      <c r="O7" s="136"/>
-      <c r="P7" s="136"/>
+      <c r="M7" s="153" t="s">
+        <v>92</v>
+      </c>
+      <c r="N7" s="153"/>
+      <c r="O7" s="153"/>
+      <c r="P7" s="153"/>
       <c r="T7">
         <f>ROUND(MAX(0,H7-(LM!B$17+LM!B$18*H7)*'CP 1. part'!P$20),2)</f>
         <v>0</v>
@@ -7503,10 +7511,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M8" s="136"/>
-      <c r="N8" s="136"/>
-      <c r="O8" s="136"/>
-      <c r="P8" s="136"/>
+      <c r="M8" s="153"/>
+      <c r="N8" s="153"/>
+      <c r="O8" s="153"/>
+      <c r="P8" s="153"/>
       <c r="T8">
         <f>ROUND(MAX(0,H8-(LM!B$17+LM!B$18*H8)*'CP 1. part'!P$20),2)</f>
         <v>0</v>
@@ -7547,10 +7555,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M9" s="136"/>
-      <c r="N9" s="136"/>
-      <c r="O9" s="136"/>
-      <c r="P9" s="136"/>
+      <c r="M9" s="153"/>
+      <c r="N9" s="153"/>
+      <c r="O9" s="153"/>
+      <c r="P9" s="153"/>
       <c r="T9">
         <f>ROUND(MAX(0,H9-(LM!B$17+LM!B$18*H9)*'CP 1. part'!P$20),2)</f>
         <v>0</v>
@@ -7591,10 +7599,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M10" s="136"/>
-      <c r="N10" s="136"/>
-      <c r="O10" s="136"/>
-      <c r="P10" s="136"/>
+      <c r="M10" s="153"/>
+      <c r="N10" s="153"/>
+      <c r="O10" s="153"/>
+      <c r="P10" s="153"/>
       <c r="T10">
         <f>ROUND(MAX(0,H10-(LM!B$17+LM!B$18*H10)*'CP 1. part'!P$20),2)</f>
         <v>0</v>
@@ -7635,10 +7643,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M11" s="136"/>
-      <c r="N11" s="136"/>
-      <c r="O11" s="136"/>
-      <c r="P11" s="136"/>
+      <c r="M11" s="153"/>
+      <c r="N11" s="153"/>
+      <c r="O11" s="153"/>
+      <c r="P11" s="153"/>
       <c r="T11">
         <f>ROUND(MAX(0,H11-(LM!B$17+LM!B$18*H11)*'CP 1. part'!P$20),2)</f>
         <v>0</v>
@@ -7679,10 +7687,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M12" s="136"/>
-      <c r="N12" s="136"/>
-      <c r="O12" s="136"/>
-      <c r="P12" s="136"/>
+      <c r="M12" s="153"/>
+      <c r="N12" s="153"/>
+      <c r="O12" s="153"/>
+      <c r="P12" s="153"/>
       <c r="T12">
         <f>ROUND(MAX(0,H12-(LM!B$17+LM!B$18*H12)*'CP 1. part'!P$20),2)</f>
         <v>1.4</v>
@@ -7723,10 +7731,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M13" s="136"/>
-      <c r="N13" s="136"/>
-      <c r="O13" s="136"/>
-      <c r="P13" s="136"/>
+      <c r="M13" s="153"/>
+      <c r="N13" s="153"/>
+      <c r="O13" s="153"/>
+      <c r="P13" s="153"/>
       <c r="T13">
         <f>ROUND(MAX(0,H13-(LM!B$17+LM!B$18*H13)*'CP 1. part'!P$20),2)</f>
         <v>0</v>
@@ -7767,10 +7775,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M14" s="136"/>
-      <c r="N14" s="136"/>
-      <c r="O14" s="136"/>
-      <c r="P14" s="136"/>
+      <c r="M14" s="153"/>
+      <c r="N14" s="153"/>
+      <c r="O14" s="153"/>
+      <c r="P14" s="153"/>
       <c r="T14">
         <f>ROUND(MAX(0,H14-(LM!B$17+LM!B$18*H14)*'CP 1. part'!P$20),2)</f>
         <v>0</v>
@@ -7811,10 +7819,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M15" s="136"/>
-      <c r="N15" s="136"/>
-      <c r="O15" s="136"/>
-      <c r="P15" s="136"/>
+      <c r="M15" s="153"/>
+      <c r="N15" s="153"/>
+      <c r="O15" s="153"/>
+      <c r="P15" s="153"/>
       <c r="T15">
         <f>ROUND(MAX(0,H15-(LM!B$17+LM!B$18*H15)*'CP 1. part'!P$20),2)</f>
         <v>6.88</v>
@@ -7855,10 +7863,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M16" s="136"/>
-      <c r="N16" s="136"/>
-      <c r="O16" s="136"/>
-      <c r="P16" s="136"/>
+      <c r="M16" s="153"/>
+      <c r="N16" s="153"/>
+      <c r="O16" s="153"/>
+      <c r="P16" s="153"/>
       <c r="T16">
         <f>ROUND(MAX(0,H16-(LM!B$17+LM!B$18*H16)*'CP 1. part'!P$20),2)</f>
         <v>1.05</v>
@@ -7899,10 +7907,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M17" s="136"/>
-      <c r="N17" s="136"/>
-      <c r="O17" s="136"/>
-      <c r="P17" s="136"/>
+      <c r="M17" s="153"/>
+      <c r="N17" s="153"/>
+      <c r="O17" s="153"/>
+      <c r="P17" s="153"/>
       <c r="T17">
         <f>ROUND(MAX(0,H17-(LM!B$17+LM!B$18*H17)*'CP 1. part'!P$20),2)</f>
         <v>0</v>
@@ -7943,10 +7951,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M18" s="136"/>
-      <c r="N18" s="136"/>
-      <c r="O18" s="136"/>
-      <c r="P18" s="136"/>
+      <c r="M18" s="153"/>
+      <c r="N18" s="153"/>
+      <c r="O18" s="153"/>
+      <c r="P18" s="153"/>
       <c r="T18">
         <f>ROUND(MAX(0,H18-(LM!B$17+LM!B$18*H18)*'CP 1. part'!P$20),2)</f>
         <v>0</v>
@@ -7987,10 +7995,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M19" s="136"/>
-      <c r="N19" s="136"/>
-      <c r="O19" s="136"/>
-      <c r="P19" s="136"/>
+      <c r="M19" s="153"/>
+      <c r="N19" s="153"/>
+      <c r="O19" s="153"/>
+      <c r="P19" s="153"/>
       <c r="T19">
         <f>ROUND(MAX(0,H19-(LM!B$17+LM!B$18*H19)*'CP 1. part'!P$20),2)</f>
         <v>0</v>
@@ -8031,10 +8039,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M20" s="136"/>
-      <c r="N20" s="136"/>
-      <c r="O20" s="136"/>
-      <c r="P20" s="136"/>
+      <c r="M20" s="153"/>
+      <c r="N20" s="153"/>
+      <c r="O20" s="153"/>
+      <c r="P20" s="153"/>
       <c r="T20">
         <f>ROUND(MAX(0,H20-(LM!B$17+LM!B$18*H20)*'CP 1. part'!P$20),2)</f>
         <v>9.16</v>
@@ -8927,29 +8935,32 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648CB31B-766B-41E0-BE25-19C52607D12B}">
-  <dimension ref="B4:U44"/>
+  <dimension ref="B4:X44"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AB29" sqref="AB29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="4" max="6" width="5.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" customWidth="1"/>
+    <col min="10" max="10" width="7" customWidth="1"/>
     <col min="13" max="13" width="4.6640625" customWidth="1"/>
-    <col min="16" max="16" width="16" customWidth="1"/>
-    <col min="17" max="18" width="7" customWidth="1"/>
-    <col min="19" max="19" width="10.21875" customWidth="1"/>
-    <col min="20" max="20" width="6.6640625" customWidth="1"/>
-    <col min="21" max="21" width="6.88671875" customWidth="1"/>
+    <col min="16" max="16" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.33203125" customWidth="1"/>
+    <col min="18" max="18" width="7.88671875" customWidth="1"/>
+    <col min="19" max="19" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.5546875" customWidth="1"/>
+    <col min="21" max="21" width="7.77734375" customWidth="1"/>
+    <col min="22" max="22" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="3:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C5" s="77" t="s">
         <v>0</v>
       </c>
@@ -8962,14 +8973,11 @@
       <c r="F5" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="79" t="b">
-        <v>1</v>
-      </c>
-      <c r="N5" s="105" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="3:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G5" s="173" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C6" s="71">
         <v>1</v>
       </c>
@@ -8985,11 +8993,11 @@
       <c r="G6" s="72">
         <v>8.4499999999999993</v>
       </c>
-      <c r="N6" s="105" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="3:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M6" s="105" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C7" s="71">
         <v>2</v>
       </c>
@@ -9005,11 +9013,11 @@
       <c r="G7" s="72">
         <v>9.25</v>
       </c>
-      <c r="N7" s="105" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="3:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M7" s="105" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="71">
         <v>3</v>
       </c>
@@ -9025,11 +9033,11 @@
       <c r="G8" s="72">
         <v>0</v>
       </c>
-      <c r="N8" s="105" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="3:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M8" s="105" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C9" s="71">
         <v>4</v>
       </c>
@@ -9045,11 +9053,11 @@
       <c r="G9" s="72">
         <v>0</v>
       </c>
-      <c r="N9" s="105" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="M9" s="105" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C10" s="71">
         <v>5</v>
       </c>
@@ -9065,8 +9073,11 @@
       <c r="G10" s="72">
         <v>9.3800000000000008</v>
       </c>
-    </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="M10" s="105" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C11" s="71">
         <v>6</v>
       </c>
@@ -9082,8 +9093,11 @@
       <c r="G11" s="72">
         <v>3.65</v>
       </c>
-    </row>
-    <row r="12" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M11" s="105" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="71">
         <v>7</v>
       </c>
@@ -9100,7 +9114,7 @@
         <v>18.940000000000001</v>
       </c>
     </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C13" s="71">
         <v>8</v>
       </c>
@@ -9116,12 +9130,12 @@
       <c r="G13" s="72">
         <v>4.83</v>
       </c>
-      <c r="K13" s="137" t="s">
+      <c r="K13" s="154" t="s">
         <v>60</v>
       </c>
-      <c r="L13" s="138"/>
-    </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="L13" s="155"/>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C14" s="71">
         <v>9</v>
       </c>
@@ -9137,10 +9151,10 @@
       <c r="G14" s="72">
         <v>0</v>
       </c>
-      <c r="K14" s="139"/>
-      <c r="L14" s="140"/>
-    </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="K14" s="156"/>
+      <c r="L14" s="157"/>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C15" s="71">
         <v>10</v>
       </c>
@@ -9156,10 +9170,10 @@
       <c r="G15" s="72">
         <v>28.8</v>
       </c>
-      <c r="K15" s="139"/>
-      <c r="L15" s="140"/>
-    </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="K15" s="156"/>
+      <c r="L15" s="157"/>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C16" s="71">
         <v>11</v>
       </c>
@@ -9175,10 +9189,10 @@
       <c r="G16" s="72">
         <v>5.65</v>
       </c>
-      <c r="K16" s="139"/>
-      <c r="L16" s="140"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="K16" s="156"/>
+      <c r="L16" s="157"/>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.3">
       <c r="C17" s="71">
         <v>12</v>
       </c>
@@ -9194,10 +9208,10 @@
       <c r="G17" s="72">
         <v>0.05</v>
       </c>
-      <c r="K17" s="139"/>
-      <c r="L17" s="140"/>
-    </row>
-    <row r="18" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K17" s="156"/>
+      <c r="L17" s="157"/>
+    </row>
+    <row r="18" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="71">
         <v>13</v>
       </c>
@@ -9213,10 +9227,10 @@
       <c r="G18" s="72">
         <v>3.27</v>
       </c>
-      <c r="K18" s="141"/>
-      <c r="L18" s="142"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="K18" s="158"/>
+      <c r="L18" s="159"/>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.3">
       <c r="C19" s="71">
         <v>14</v>
       </c>
@@ -9237,7 +9251,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.3">
       <c r="C20" s="71">
         <v>15</v>
       </c>
@@ -9260,7 +9274,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="2:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:24" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="73">
         <v>16</v>
       </c>
@@ -9283,25 +9297,34 @@
         <v>1</v>
       </c>
       <c r="P21" s="96" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q21" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="Q21" s="97" t="s">
+      <c r="R21" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="R21" s="98" t="s">
-        <v>69</v>
-      </c>
       <c r="S21" s="99" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="T21" s="100" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="U21" s="101" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="V21" s="175" t="s">
+        <v>106</v>
+      </c>
+      <c r="W21" s="176" t="s">
+        <v>102</v>
+      </c>
+      <c r="X21" s="177" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.3">
       <c r="N22" s="26">
         <v>1</v>
       </c>
@@ -9330,8 +9353,17 @@
         <f>IF(O22&lt;S22,1,0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="V22" s="178" t="s">
+        <v>25</v>
+      </c>
+      <c r="W22" s="179" t="s">
+        <v>25</v>
+      </c>
+      <c r="X22" s="180" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.3">
       <c r="N23" s="28">
         <v>2</v>
       </c>
@@ -9360,8 +9392,11 @@
         <f t="shared" ref="U23:U37" si="3">IF(O23&lt;S23,1,0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V23" s="178"/>
+      <c r="W23" s="179"/>
+      <c r="X23" s="180"/>
+    </row>
+    <row r="24" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N24" s="28">
         <v>3</v>
       </c>
@@ -9390,8 +9425,11 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="V24" s="178"/>
+      <c r="W24" s="179"/>
+      <c r="X24" s="180"/>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B25" s="60" t="s">
         <v>63</v>
       </c>
@@ -9441,8 +9479,11 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="V25" s="178"/>
+      <c r="W25" s="179"/>
+      <c r="X25" s="180"/>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B26" s="63">
         <v>1</v>
       </c>
@@ -9494,8 +9535,11 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="V26" s="178"/>
+      <c r="W26" s="179"/>
+      <c r="X26" s="180"/>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B27" s="66">
         <v>2</v>
       </c>
@@ -9547,8 +9591,11 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="V27" s="178"/>
+      <c r="W27" s="179"/>
+      <c r="X27" s="180"/>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B28" s="54">
         <v>3</v>
       </c>
@@ -9568,8 +9615,8 @@
         <v>1.2E-4</v>
       </c>
       <c r="H28" s="59">
-        <f t="shared" ref="G28:H29" ca="1" si="4">RAND()</f>
-        <v>0.61698554823039142</v>
+        <f ca="1">RAND()</f>
+        <v>0.19620510287109383</v>
       </c>
       <c r="N28" s="28">
         <v>7</v>
@@ -9599,8 +9646,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="V28" s="178"/>
+      <c r="W28" s="179"/>
+      <c r="X28" s="180"/>
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B29" s="54">
         <v>4</v>
       </c>
@@ -9617,8 +9667,8 @@
         <v>0.5</v>
       </c>
       <c r="G29" s="58">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.73405916343569688</v>
+        <f t="shared" ref="G28:H29" ca="1" si="4">RAND()</f>
+        <v>0.54249040798491255</v>
       </c>
       <c r="H29" s="102">
         <v>4.2099999999999999E-2</v>
@@ -9651,8 +9701,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="V29" s="178"/>
+      <c r="W29" s="179"/>
+      <c r="X29" s="180"/>
+    </row>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B30" s="54" t="s">
         <v>20</v>
       </c>
@@ -9702,8 +9755,11 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="V30" s="178"/>
+      <c r="W30" s="179"/>
+      <c r="X30" s="180"/>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B31" s="54" t="s">
         <v>20</v>
       </c>
@@ -9753,8 +9809,11 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="V31" s="178"/>
+      <c r="W31" s="179"/>
+      <c r="X31" s="180"/>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B32" s="54" t="s">
         <v>20</v>
       </c>
@@ -9804,10 +9863,13 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="56" t="s">
-        <v>20</v>
+      <c r="V32" s="178"/>
+      <c r="W32" s="179"/>
+      <c r="X32" s="180"/>
+    </row>
+    <row r="33" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="174" t="s">
+        <v>94</v>
       </c>
       <c r="C33" s="56" t="s">
         <v>20</v>
@@ -9855,8 +9917,11 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="V33" s="178"/>
+      <c r="W33" s="179"/>
+      <c r="X33" s="180"/>
+    </row>
+    <row r="34" spans="2:24" x14ac:dyDescent="0.3">
       <c r="N34" s="28">
         <v>13</v>
       </c>
@@ -9885,8 +9950,11 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="V34" s="178"/>
+      <c r="W34" s="179"/>
+      <c r="X34" s="180"/>
+    </row>
+    <row r="35" spans="2:24" x14ac:dyDescent="0.3">
       <c r="F35" t="s">
         <v>66</v>
       </c>
@@ -9926,8 +9994,11 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V35" s="178"/>
+      <c r="W35" s="179"/>
+      <c r="X35" s="180"/>
+    </row>
+    <row r="36" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N36" s="28">
         <v>15</v>
       </c>
@@ -9956,17 +10027,20 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="V36" s="178"/>
+      <c r="W36" s="179"/>
+      <c r="X36" s="180"/>
+    </row>
+    <row r="37" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B37" s="119" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C37" s="53"/>
       <c r="D37" s="53"/>
       <c r="E37" s="53"/>
       <c r="F37" s="53"/>
       <c r="G37" s="76" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N37" s="30">
         <v>16</v>
@@ -9996,17 +10070,20 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V37" s="181"/>
+      <c r="W37" s="182"/>
+      <c r="X37" s="183"/>
+    </row>
+    <row r="38" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="56" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C38" s="43"/>
       <c r="D38" s="43"/>
       <c r="E38" s="43"/>
       <c r="F38" s="43"/>
       <c r="G38" s="104" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P38" t="s">
         <v>64</v>
@@ -10027,8 +10104,14 @@
         <f>AVERAGE(U22:U37)</f>
         <v>0.8125</v>
       </c>
-    </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="W38" t="s">
+        <v>25</v>
+      </c>
+      <c r="X38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="2:24" x14ac:dyDescent="0.3">
       <c r="P39" t="s">
         <v>65</v>
       </c>
@@ -10049,27 +10132,27 @@
         <v>0.76249999999999996</v>
       </c>
     </row>
-    <row r="41" spans="2:21" ht="18" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:24" ht="18" x14ac:dyDescent="0.35">
       <c r="K41" s="118" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="L41" s="117" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="2:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="L42" s="105" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="L43" s="41" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="L44" t="s">
-        <v>86</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="2:24" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L43" s="117" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="2:24" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L44" s="117" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -10085,8 +10168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A5C9D6-2333-41E8-97C6-9FADE584365B}">
   <dimension ref="C4:V33"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10099,25 +10182,25 @@
   <sheetData>
     <row r="4" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C5" s="143" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="144"/>
-      <c r="E5" s="144"/>
-      <c r="F5" s="144"/>
+      <c r="C5" s="160" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
       <c r="G5" s="112" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="162" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="113" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="145" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="146"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="146"/>
-      <c r="G6" s="113" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -10141,13 +10224,13 @@
         <v>1</v>
       </c>
       <c r="O8" s="114" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="P8" s="78" t="s">
         <v>62</v>
       </c>
       <c r="Q8" s="109" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="R8" s="79" t="s">
         <v>61</v>
@@ -10221,7 +10304,7 @@
         <v>1</v>
       </c>
       <c r="V10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="3:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10271,11 +10354,11 @@
       <c r="F12" s="72">
         <v>747</v>
       </c>
-      <c r="I12" s="147" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" s="148"/>
-      <c r="K12" s="149"/>
+      <c r="I12" s="164" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" s="165"/>
+      <c r="K12" s="166"/>
       <c r="M12" s="107">
         <v>5003</v>
       </c>
@@ -10310,9 +10393,9 @@
       <c r="F13" s="72">
         <v>305</v>
       </c>
-      <c r="I13" s="150"/>
-      <c r="J13" s="151"/>
-      <c r="K13" s="152"/>
+      <c r="I13" s="167"/>
+      <c r="J13" s="168"/>
+      <c r="K13" s="169"/>
       <c r="M13" s="107">
         <v>5004</v>
       </c>
@@ -10347,9 +10430,9 @@
       <c r="F14" s="72">
         <v>770</v>
       </c>
-      <c r="I14" s="150"/>
-      <c r="J14" s="151"/>
-      <c r="K14" s="152"/>
+      <c r="I14" s="167"/>
+      <c r="J14" s="168"/>
+      <c r="K14" s="169"/>
       <c r="M14" s="107">
         <v>5005</v>
       </c>
@@ -10384,9 +10467,9 @@
       <c r="F15" s="72">
         <v>175</v>
       </c>
-      <c r="I15" s="150"/>
-      <c r="J15" s="151"/>
-      <c r="K15" s="152"/>
+      <c r="I15" s="167"/>
+      <c r="J15" s="168"/>
+      <c r="K15" s="169"/>
       <c r="M15" s="107">
         <v>5006</v>
       </c>
@@ -10421,9 +10504,9 @@
       <c r="F16" s="72">
         <v>247</v>
       </c>
-      <c r="I16" s="153"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="155"/>
+      <c r="I16" s="170"/>
+      <c r="J16" s="171"/>
+      <c r="K16" s="172"/>
       <c r="M16" s="107">
         <v>5007</v>
       </c>
@@ -10733,30 +10816,30 @@
     </row>
     <row r="27" spans="3:18" x14ac:dyDescent="0.3">
       <c r="O27" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="3:18" x14ac:dyDescent="0.3">
       <c r="I29" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="3:18" x14ac:dyDescent="0.3">
       <c r="I30" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="3:18" x14ac:dyDescent="0.3">
       <c r="I31" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="9:10" ht="18" x14ac:dyDescent="0.35">
       <c r="I33" s="118" t="s">
+        <v>74</v>
+      </c>
+      <c r="J33" t="s">
         <v>82</v>
-      </c>
-      <c r="J33" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>